<commit_message>
add params numerosity for type options parameters, typo fixed to disambiguate IRP/IRV order
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -1235,7 +1235,9 @@
     <t>Residential</t>
   </si>
   <si>
-    <t>{"type": "options"}</t>
+    <t>{"type": "options",
+ "params_min": 0,
+ "params_max": 1}</t>
   </si>
   <si>
     <t>RES:1</t>
@@ -20066,7 +20068,7 @@
       <c r="H16" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20213,7 +20215,7 @@
       <c r="H28" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K28" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20255,7 +20257,7 @@
       <c r="H31" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20346,7 +20348,7 @@
       <c r="H38" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20394,7 +20396,7 @@
       <c r="H42" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="K42" s="19" t="s">
+      <c r="K42" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20470,7 +20472,7 @@
       <c r="H48" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="K48" s="19" t="s">
+      <c r="K48" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20595,7 +20597,7 @@
       <c r="H59" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="K59" s="19" t="s">
+      <c r="K59" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -20720,7 +20722,7 @@
       <c r="H70" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="K70" s="19" t="s">
+      <c r="K70" s="16" t="s">
         <v>363</v>
       </c>
     </row>
@@ -23194,8 +23196,8 @@
       <c r="F7" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="H7" s="8">
-        <v>0.0</v>
+      <c r="H7" s="16">
+        <v>100.0</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>627</v>

</xml_diff>

<commit_message>
add params numerosity for all parameters types
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -1023,7 +1023,9 @@
             "min": 0,
             "min_incl": true,
             "max": 1,
-            "max_incl": true
+            "max_incl": true,
+            "params_min": 1,
+            "params_max": 1
             }</t>
   </si>
   <si>
@@ -1051,7 +1053,9 @@
     <t>{
             "type": "rangeable_int",
             "min": 0,
-            "min_incl": true
+            "min_incl": true,
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>
@@ -1064,7 +1068,9 @@
     <t>{
             "type": "int",
             "min": 0,
-            "min_incl": true
+            "min_incl": true,
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>
@@ -1083,7 +1089,9 @@
     <t>{
             "type": "float",
             "min": 1,
-            "min_incl": true
+            "min_incl": true,
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>
@@ -1126,7 +1134,9 @@
     <t>{
             "type": "rangeable_float",
             "min": 0,
-            "min_incl": true
+            "min_incl": true,
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>
@@ -1139,7 +1149,9 @@
     <t>{
             "type": "float",
             "min": 0,
-            "min_incl": true
+            "min_incl": true,
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>
@@ -1160,7 +1172,9 @@
             "min": 0,
             "min_incl": true,
             "max": 90,
-            "max_incl": false
+            "max_incl": false,
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>
@@ -1180,7 +1194,9 @@
   </si>
   <si>
     <t>{
-            "type": "int"
+            "type": "int",
+            "params_min": 1,
+            "params_max": 1
 }</t>
   </si>
   <si>

</xml_diff>

<commit_message>
update Y type from int to rangeable int and some dates atoms descriptions (taxonomy 3.3)
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -23,76 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="K10">
-      <text>
-        <t xml:space="preserve">type float?
-	-Catalina YepesE</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D4">
-      <text>
-        <t xml:space="preserve">Shall we adjust the description:
-H:n, exact number of storeys above ground.
-H:a-b, range of storeys above ground.
-H:&lt;n, n number of storeys above ground or less
-H:&gt;n, n number of storeys above ground or more
-	-Catalina YepesE
-to be sure: two Taxonomies that describe two different ranges of storeys will be:
-.../H:&lt;5/...
-and
-.../H:&gt;6/...
-correct?
-	-Matteo Nastasi
-_Marked as resolved_
-	-Catalina YepesE
-_Re-opened_
-	-Catalina YepesE
-Yes, correct
-	-Catalina YepesE
-Cata, I'm sorry but I'm still strongly convinced that a new user will understand "&lt;" as "less than" and not as "less or equal than", I need to discuss more with you about it .
-	-Matteo Nastasi
-@catalina.yepes@globalquakemodel.org now H can accept ranges or limits (&lt; or &gt;) probably the description must be changed (sound me strange "exact" for a range) but just to be sure ...
-also the format maybe should be moved in the "Example" column
-	-Matteo Nastasi
-What about:
-"Number of storeys above ground. It can be an exact number or a range."
-	-Catalina YepesE
-And I like the idea of including different examples
-	-Catalina YepesE
-@catalina.yepes@globalquakemodel.org seems to me that with a so long description we must to think about the idea that we need a new field so we can split the description: "Number of storeys above ground" and the extended description as you wrote above; it seems to me more ergonomic for the future taxtweb and to have a short description of each atom when needed (or far better a "title" and an optional "description" for each of them).
-	-Matteo Nastasi
-LGTM
-	-Catalina YepesE</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="C4">
-      <text>
-        <t xml:space="preserve">Controllare se sono unique strings
-	-Catalina YepesE</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="883">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -1068,7 +1000,10 @@
     <t>HAPP</t>
   </si>
   <si>
-    <t>HAPP:n, approximate number of storeys above ground.</t>
+    <t>Approximate number of storeys above ground.</t>
+  </si>
+  <si>
+    <t>HAPP:n</t>
   </si>
   <si>
     <t>{
@@ -1089,7 +1024,10 @@
     <t>HHT</t>
   </si>
   <si>
-    <t>HHT:n, total height of the structure, measured from the ground floor. Float specifying the height of the structures in meters. (HHT&gt;= 1)</t>
+    <t>Total height of the structure, measured from the ground floor. Float specifying the height of the structures in meters. (HHT&gt;= 1)</t>
+  </si>
+  <si>
+    <t>HHT:n</t>
   </si>
   <si>
     <t>{
@@ -1104,7 +1042,10 @@
     <t>HHI</t>
   </si>
   <si>
-    <t>HHI:n, inter-storey height (average). Float specifying the average floor height in meters. (HHI&gt;= 1)</t>
+    <t>Inter-storey height (average). Float specifying the average floor height in meters. (HHI&gt;= 1)</t>
+  </si>
+  <si>
+    <t>HHI:n</t>
   </si>
   <si>
     <t>number_storeys_below</t>
@@ -1116,13 +1057,22 @@
     <t>HB</t>
   </si>
   <si>
-    <t>HB:n, exact number of storeys below ground (same as number of basements)</t>
+    <t>Number of storeys below ground (same as number of basements)</t>
+  </si>
+  <si>
+    <t>HB:n, exact number of storeys below ground.
+HB:a-b, range of storeys below ground.
+HB:&lt;n, n upper limit of number of storeys below ground (with n excluded).
+HB:&gt;n, n lower limit of number of storeys below ground (with n excluded).</t>
   </si>
   <si>
     <t>HBAPP</t>
   </si>
   <si>
-    <t>HBAPP:n, approximate number of storeys below ground</t>
+    <t>Approximate number of storeys below ground</t>
+  </si>
+  <si>
+    <t>HBAPP:n</t>
   </si>
   <si>
     <t>height_ground_floor</t>
@@ -1134,7 +1084,13 @@
     <t>HF</t>
   </si>
   <si>
-    <t>HF:n, exact height of ground floor level above grade</t>
+    <t>Height of ground floor level above grade</t>
+  </si>
+  <si>
+    <t>HF:n, exact height of ground floor above grade.
+HF:a-b, range of height of ground floor above grade.
+HF:&lt;n, n upper limit of the height of ground floor above grade. (with n excluded).
+HF:&gt;n, n lower limit of the height of ground floor above grade. (with n excluded).</t>
   </si>
   <si>
     <t>{
@@ -1149,7 +1105,10 @@
     <t>HFAPP</t>
   </si>
   <si>
-    <t>HFAPP:n, approximate height of  ground floor level above grade</t>
+    <t>Approximate height of ground floor level above grade</t>
+  </si>
+  <si>
+    <t>HFAPP:n</t>
   </si>
   <si>
     <t>{
@@ -1170,7 +1129,10 @@
     <t>HD</t>
   </si>
   <si>
-    <t>HD:n, slope of the ground (n=float in degrees).</t>
+    <t>q</t>
+  </si>
+  <si>
+    <t>HD:n</t>
   </si>
   <si>
     <t>{
@@ -1196,7 +1158,26 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Y:n, Exact date of construction or retrofit</t>
+    <t>Date of construction or retrofit</t>
+  </si>
+  <si>
+    <t>Y:n, exact date of construction or retrofit.
+Y:a-b, range of date of construction or retrofit.
+Y:&lt;n, n upper limit of date of construction or retrofit (with n excluded).
+Y:&gt;n, n lower limit of date of construction or retrofit (with n excluded).</t>
+  </si>
+  <si>
+    <t>{
+            "type": "rangeable_int",
+            "params_min": 1,
+            "params_max": 1
+}</t>
+  </si>
+  <si>
+    <t>YAPP</t>
+  </si>
+  <si>
+    <t>Approximate date of construction or retrofit</t>
   </si>
   <si>
     <t>{
@@ -1204,12 +1185,6 @@
             "params_min": 1,
             "params_max": 1
 }</t>
-  </si>
-  <si>
-    <t>YAPP</t>
-  </si>
-  <si>
-    <t>YAPP:n, Approximate date of construction or retrofit</t>
   </si>
   <si>
     <t>physical_condition_maintenance</t>
@@ -2981,14 +2956,14 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -4720,7 +4695,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4771,16 +4746,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -4788,10 +4763,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -4799,10 +4774,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>668</v>
+        <v>678</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -4810,10 +4785,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>669</v>
+        <v>679</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -4821,10 +4796,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -4832,10 +4807,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>673</v>
+        <v>683</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -4843,7 +4818,7 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>675</v>
+        <v>685</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>102</v>
@@ -4854,10 +4829,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>676</v>
+        <v>686</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>677</v>
+        <v>687</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -4865,10 +4840,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>678</v>
+        <v>688</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>679</v>
+        <v>689</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -4876,10 +4851,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>680</v>
+        <v>690</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>681</v>
+        <v>691</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -4887,10 +4862,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>682</v>
+        <v>692</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>683</v>
+        <v>693</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -4898,16 +4873,16 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>684</v>
+        <v>694</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>685</v>
+        <v>695</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>686</v>
+        <v>696</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>687</v>
+        <v>697</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>60</v>
@@ -4915,10 +4890,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>689</v>
+        <v>699</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>64</v>
@@ -4926,10 +4901,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>691</v>
+        <v>701</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>67</v>
@@ -4937,10 +4912,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>692</v>
+        <v>702</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>693</v>
+        <v>703</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>70</v>
@@ -4948,19 +4923,19 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>695</v>
+        <v>705</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>696</v>
+        <v>706</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>697</v>
+        <v>707</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>60</v>
@@ -4968,13 +4943,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>699</v>
+        <v>709</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>64</v>
@@ -6003,7 +5978,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>701</v>
+        <v>711</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6054,16 +6029,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>702</v>
+        <v>712</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>703</v>
+        <v>713</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>704</v>
+        <v>714</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>705</v>
+        <v>715</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -6071,10 +6046,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>706</v>
+        <v>716</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>707</v>
+        <v>717</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -6082,10 +6057,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>708</v>
+        <v>718</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>709</v>
+        <v>719</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -6093,10 +6068,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>710</v>
+        <v>720</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>711</v>
+        <v>721</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -6104,10 +6079,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>712</v>
+        <v>722</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>713</v>
+        <v>723</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -6115,10 +6090,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>714</v>
+        <v>724</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>715</v>
+        <v>725</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -6126,10 +6101,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>716</v>
+        <v>726</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>717</v>
+        <v>727</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -6137,10 +6112,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>718</v>
+        <v>728</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>719</v>
+        <v>729</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -6148,10 +6123,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>720</v>
+        <v>730</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>721</v>
+        <v>731</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -6159,10 +6134,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>722</v>
+        <v>732</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>723</v>
+        <v>733</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -6170,16 +6145,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>725</v>
+        <v>735</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>726</v>
+        <v>736</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>727</v>
+        <v>737</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>60</v>
@@ -6187,10 +6162,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>728</v>
+        <v>738</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>729</v>
+        <v>739</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>64</v>
@@ -6198,10 +6173,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>730</v>
+        <v>740</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>731</v>
+        <v>741</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>67</v>
@@ -6209,10 +6184,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>732</v>
+        <v>742</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>733</v>
+        <v>743</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>70</v>
@@ -6220,7 +6195,7 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>214</v>
@@ -6231,10 +6206,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>735</v>
+        <v>745</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>736</v>
+        <v>746</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>76</v>
@@ -6242,10 +6217,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>737</v>
+        <v>747</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>79</v>
@@ -6253,10 +6228,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>739</v>
+        <v>749</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>740</v>
+        <v>750</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>82</v>
@@ -6264,10 +6239,10 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>741</v>
+        <v>751</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>674</v>
+        <v>684</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>85</v>
@@ -6275,10 +6250,10 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>742</v>
+        <v>752</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>88</v>
@@ -6286,10 +6261,10 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>745</v>
+        <v>755</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>91</v>
@@ -6297,10 +6272,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>746</v>
+        <v>756</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>747</v>
+        <v>757</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>94</v>
@@ -6308,10 +6283,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>748</v>
+        <v>758</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>749</v>
+        <v>759</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>97</v>
@@ -6319,16 +6294,16 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>750</v>
+        <v>760</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>751</v>
+        <v>761</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>60</v>
@@ -6336,10 +6311,10 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>753</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>743</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>64</v>
@@ -6347,10 +6322,10 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="8" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>67</v>
@@ -6358,10 +6333,10 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="8" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>756</v>
+        <v>766</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>70</v>
@@ -6369,7 +6344,7 @@
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>102</v>
@@ -6380,10 +6355,10 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="8" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>76</v>
@@ -6391,10 +6366,10 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="8" t="s">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>79</v>
@@ -6402,19 +6377,19 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>774</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>775</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>762</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>763</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>764</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>765</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>752</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>60</v>
@@ -6422,13 +6397,13 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="8" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>64</v>
@@ -6436,13 +6411,13 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="8" t="s">
-        <v>768</v>
+        <v>778</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>769</v>
+        <v>779</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>67</v>
@@ -6450,13 +6425,13 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="8" t="s">
-        <v>770</v>
+        <v>780</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>771</v>
+        <v>781</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>753</v>
+        <v>763</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>70</v>
@@ -6464,13 +6439,13 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
-        <v>772</v>
+        <v>782</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>773</v>
+        <v>783</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>73</v>
@@ -6478,13 +6453,13 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
-        <v>774</v>
+        <v>784</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>775</v>
+        <v>785</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>76</v>
@@ -6492,13 +6467,13 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
-        <v>776</v>
+        <v>786</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>777</v>
+        <v>787</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>79</v>
@@ -6506,13 +6481,13 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
-        <v>778</v>
+        <v>788</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>779</v>
+        <v>789</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>82</v>
@@ -6520,13 +6495,13 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>780</v>
+        <v>790</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>781</v>
+        <v>791</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>85</v>
@@ -6534,13 +6509,13 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
-        <v>782</v>
+        <v>792</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>783</v>
+        <v>793</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>88</v>
@@ -6548,13 +6523,13 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
-        <v>784</v>
+        <v>794</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>785</v>
+        <v>795</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>91</v>
@@ -6562,13 +6537,13 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="8" t="s">
-        <v>786</v>
+        <v>796</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>787</v>
+        <v>797</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>94</v>
@@ -6576,13 +6551,13 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="8" t="s">
-        <v>788</v>
+        <v>798</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>789</v>
+        <v>799</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>97</v>
@@ -6590,13 +6565,13 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="8" t="s">
-        <v>790</v>
+        <v>800</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>791</v>
+        <v>801</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>100</v>
@@ -6604,13 +6579,13 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
-        <v>792</v>
+        <v>802</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>793</v>
+        <v>803</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>103</v>
@@ -6618,13 +6593,13 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
-        <v>794</v>
+        <v>804</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>795</v>
+        <v>805</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>106</v>
@@ -6632,13 +6607,13 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
-        <v>796</v>
+        <v>806</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>797</v>
+        <v>807</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>110</v>
@@ -6646,13 +6621,13 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>798</v>
+        <v>808</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>799</v>
+        <v>809</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>758</v>
+        <v>768</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>113</v>
@@ -6660,16 +6635,16 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>800</v>
+        <v>810</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>801</v>
+        <v>811</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>802</v>
+        <v>812</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>803</v>
+        <v>813</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>60</v>
@@ -6677,10 +6652,10 @@
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>804</v>
+        <v>814</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>805</v>
+        <v>815</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>64</v>
@@ -6688,10 +6663,10 @@
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>806</v>
+        <v>816</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>807</v>
+        <v>817</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>67</v>
@@ -6699,10 +6674,10 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>808</v>
+        <v>818</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>809</v>
+        <v>819</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>70</v>
@@ -7700,7 +7675,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>810</v>
+        <v>820</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7751,16 +7726,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>811</v>
+        <v>821</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>812</v>
+        <v>822</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>813</v>
+        <v>823</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>814</v>
+        <v>824</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -7768,10 +7743,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>815</v>
+        <v>825</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -7779,10 +7754,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>816</v>
+        <v>826</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -7790,10 +7765,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -7801,10 +7776,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>672</v>
+        <v>682</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -7812,7 +7787,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>102</v>
@@ -7823,10 +7798,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>820</v>
+        <v>830</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>821</v>
+        <v>831</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -7834,19 +7809,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>822</v>
+        <v>832</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>823</v>
+        <v>833</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>824</v>
+        <v>834</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>765</v>
+        <v>775</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>815</v>
+        <v>825</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -7854,13 +7829,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
+        <v>835</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>825</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>767</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>815</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -7868,13 +7843,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>826</v>
+        <v>836</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>827</v>
+        <v>837</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>815</v>
+        <v>825</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -7882,13 +7857,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>828</v>
+        <v>838</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>829</v>
+        <v>839</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -7896,13 +7871,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>830</v>
+        <v>840</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>831</v>
+        <v>841</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -7910,13 +7885,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>832</v>
+        <v>842</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>833</v>
+        <v>843</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -7924,13 +7899,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>834</v>
+        <v>844</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>835</v>
+        <v>845</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -7938,13 +7913,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>836</v>
+        <v>846</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>837</v>
+        <v>847</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>82</v>
@@ -7952,13 +7927,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>838</v>
+        <v>848</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>839</v>
+        <v>849</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>85</v>
@@ -7966,13 +7941,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>840</v>
+        <v>850</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>785</v>
+        <v>795</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>88</v>
@@ -7980,13 +7955,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>841</v>
+        <v>851</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>842</v>
+        <v>852</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>91</v>
@@ -7994,13 +7969,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>843</v>
+        <v>853</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>844</v>
+        <v>854</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>94</v>
@@ -8008,13 +7983,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>845</v>
+        <v>855</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>846</v>
+        <v>856</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>97</v>
@@ -8022,13 +7997,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>847</v>
+        <v>857</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>848</v>
+        <v>858</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>100</v>
@@ -8036,16 +8011,16 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>849</v>
+        <v>859</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>850</v>
+        <v>860</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>851</v>
+        <v>861</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>852</v>
+        <v>862</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>60</v>
@@ -8053,10 +8028,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>853</v>
+        <v>863</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>854</v>
+        <v>864</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>64</v>
@@ -9078,7 +9053,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>855</v>
+        <v>865</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9129,16 +9104,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>856</v>
+        <v>866</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>857</v>
+        <v>867</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>858</v>
+        <v>868</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -9146,10 +9121,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>859</v>
+        <v>869</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>860</v>
+        <v>870</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -9157,10 +9132,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>861</v>
+        <v>871</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>862</v>
+        <v>872</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -9168,10 +9143,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>863</v>
+        <v>873</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>864</v>
+        <v>874</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -9179,10 +9154,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>865</v>
+        <v>875</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>866</v>
+        <v>876</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -10218,7 +10193,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>867</v>
+        <v>877</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10269,16 +10244,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>868</v>
+        <v>878</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>869</v>
+        <v>879</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>870</v>
+        <v>880</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -10286,10 +10261,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>871</v>
+        <v>881</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>872</v>
+        <v>882</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -45414,67 +45389,75 @@
       <c r="C5" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="30" t="s">
+        <v>313</v>
+      </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="D6" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="D6" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>319</v>
+      </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>320</v>
-      </c>
-      <c r="E7" s="24"/>
+        <v>321</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>323</v>
+      </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>324</v>
-      </c>
-      <c r="E8" s="24"/>
+        <v>326</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>328</v>
+      </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
       </c>
@@ -45484,74 +45467,82 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="E9" s="24"/>
+        <v>329</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>331</v>
+      </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>330</v>
-      </c>
-      <c r="E10" s="24"/>
+        <v>334</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>336</v>
+      </c>
       <c r="H10" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>333</v>
-      </c>
-      <c r="E11" s="24"/>
+        <v>338</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>340</v>
+      </c>
       <c r="H11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>338</v>
-      </c>
-      <c r="E12" s="24"/>
+        <v>344</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>346</v>
+      </c>
       <c r="H12" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
@@ -49521,8 +49512,7 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -49540,19 +49530,19 @@
     <col customWidth="1" min="2" max="2" width="30.29"/>
     <col customWidth="1" min="3" max="3" width="11.43"/>
     <col customWidth="1" min="4" max="4" width="48.43"/>
-    <col customWidth="1" min="5" max="5" width="16.29"/>
+    <col customWidth="1" min="5" max="5" width="61.0"/>
     <col customWidth="1" min="6" max="6" width="13.71"/>
     <col customWidth="1" min="7" max="7" width="8.43"/>
     <col customWidth="1" min="8" max="8" width="5.0"/>
     <col customWidth="1" min="9" max="9" width="5.29"/>
     <col customWidth="1" min="10" max="10" width="13.43"/>
-    <col customWidth="1" min="11" max="11" width="20.29"/>
+    <col customWidth="1" min="11" max="11" width="27.29"/>
     <col customWidth="1" min="12" max="27" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -49603,50 +49593,53 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>344</v>
+        <v>351</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>353</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>347</v>
+        <v>355</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>356</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>67</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
@@ -49654,10 +49647,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
@@ -49665,10 +49658,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>67</v>
@@ -50706,7 +50699,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -50733,7 +50726,7 @@
       <c r="D3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="31" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -50757,31 +50750,31 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>358</v>
+        <v>367</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>368</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="E4" s="29"/>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -50789,10 +50782,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -50800,10 +50793,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -50811,10 +50804,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -50822,10 +50815,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -50833,10 +50826,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -50844,10 +50837,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -50855,10 +50848,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -50866,10 +50859,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -50877,10 +50870,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -50888,10 +50881,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -50899,25 +50892,25 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="29" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="E16" s="29"/>
       <c r="H16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="29" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="E17" s="29"/>
       <c r="H17" s="8" t="s">
@@ -50926,10 +50919,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="29" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="E18" s="29"/>
       <c r="H18" s="8" t="s">
@@ -50938,10 +50931,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="29" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="E19" s="29"/>
       <c r="H19" s="8" t="s">
@@ -50950,10 +50943,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="29" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="E20" s="29"/>
       <c r="H20" s="8" t="s">
@@ -50962,10 +50955,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="29" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="E21" s="29"/>
       <c r="H21" s="8" t="s">
@@ -50974,640 +50967,640 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="29" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="E22" s="29"/>
       <c r="H22" s="8" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="29" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="E23" s="29"/>
       <c r="H23" s="8" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="29" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="E24" s="29"/>
       <c r="H24" s="8" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="29" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="E25" s="29"/>
       <c r="H25" s="8" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="29" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="E26" s="29"/>
       <c r="H26" s="8" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="29" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="E27" s="29"/>
       <c r="H27" s="8" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="29" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="E28" s="29"/>
       <c r="H28" s="8" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="29" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E29" s="29"/>
       <c r="H29" s="8" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="29" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="E30" s="29"/>
       <c r="H30" s="8" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="E31" s="29"/>
       <c r="H31" s="8" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="K31" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="29" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="E32" s="29"/>
       <c r="H32" s="8" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="29" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="E33" s="29"/>
       <c r="H33" s="8" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="C34" s="29" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="E34" s="29"/>
       <c r="H34" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="K34" s="32"/>
+        <v>445</v>
+      </c>
+      <c r="K34" s="30"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="29" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="E35" s="29"/>
       <c r="H35" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="K35" s="32"/>
+        <v>448</v>
+      </c>
+      <c r="K35" s="30"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="29" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="E36" s="29"/>
       <c r="H36" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="K36" s="32"/>
+        <v>451</v>
+      </c>
+      <c r="K36" s="30"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="29" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="E37" s="29"/>
       <c r="H37" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="K37" s="32"/>
+        <v>454</v>
+      </c>
+      <c r="K37" s="30"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="E38" s="29"/>
       <c r="H38" s="8" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="E42" s="29"/>
       <c r="H42" s="8" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="K42" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="29" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>467</v>
+        <v>477</v>
       </c>
       <c r="E45" s="29"/>
       <c r="H45" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="K45" s="32"/>
+        <v>478</v>
+      </c>
+      <c r="K45" s="30"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="29" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="E46" s="29"/>
       <c r="H46" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="K46" s="32"/>
+        <v>481</v>
+      </c>
+      <c r="K46" s="30"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="29" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="E47" s="29"/>
       <c r="H47" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="K47" s="32"/>
+        <v>484</v>
+      </c>
+      <c r="K47" s="30"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="E48" s="29"/>
       <c r="H48" s="8" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="K48" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>479</v>
+        <v>489</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>480</v>
+        <v>490</v>
       </c>
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>482</v>
+        <v>492</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>484</v>
+        <v>494</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>486</v>
+        <v>496</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="C52" s="8" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>491</v>
+        <v>501</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>492</v>
+        <v>502</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>493</v>
+        <v>503</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>495</v>
+        <v>505</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1">
       <c r="C56" s="8" t="s">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="C57" s="8" t="s">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
     </row>
     <row r="58" ht="13.5" customHeight="1">
       <c r="C58" s="8" t="s">
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
       <c r="C59" s="8" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>509</v>
+        <v>519</v>
       </c>
       <c r="E59" s="29"/>
       <c r="H59" s="8" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="60" ht="13.5" customHeight="1">
       <c r="C60" s="8" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>513</v>
+        <v>523</v>
       </c>
     </row>
     <row r="61" ht="13.5" customHeight="1">
       <c r="C61" s="8" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>516</v>
+        <v>526</v>
       </c>
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="C62" s="8" t="s">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="C63" s="8" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
     </row>
     <row r="64" ht="13.5" customHeight="1">
       <c r="C64" s="8" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
     </row>
     <row r="65" ht="13.5" customHeight="1">
       <c r="C65" s="8" t="s">
-        <v>526</v>
+        <v>536</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>527</v>
+        <v>537</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
     </row>
     <row r="66" ht="13.5" customHeight="1">
       <c r="C66" s="8" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="C67" s="8" t="s">
-        <v>532</v>
+        <v>542</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>533</v>
+        <v>543</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="C68" s="8" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>537</v>
+        <v>547</v>
       </c>
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="C69" s="8" t="s">
-        <v>538</v>
+        <v>548</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>539</v>
+        <v>549</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>540</v>
+        <v>550</v>
       </c>
     </row>
     <row r="70" ht="13.5" customHeight="1">
       <c r="C70" s="29" t="s">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>542</v>
+        <v>552</v>
       </c>
       <c r="E70" s="29"/>
       <c r="H70" s="8" t="s">
-        <v>543</v>
+        <v>553</v>
       </c>
       <c r="K70" s="29" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="C71" s="29" t="s">
-        <v>544</v>
+        <v>554</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="E71" s="29"/>
       <c r="H71" s="8" t="s">
-        <v>546</v>
+        <v>556</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="C72" s="29" t="s">
-        <v>547</v>
+        <v>557</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>548</v>
+        <v>558</v>
       </c>
       <c r="E72" s="29"/>
       <c r="H72" s="8" t="s">
-        <v>549</v>
+        <v>559</v>
       </c>
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="C73" s="29" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="E73" s="29"/>
       <c r="H73" s="8" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
     </row>
     <row r="74" ht="13.5" customHeight="1">
       <c r="C74" s="8" t="s">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>555</v>
+        <v>565</v>
       </c>
     </row>
     <row r="75" ht="13.5" customHeight="1"/>
@@ -52577,7 +52570,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>556</v>
+        <v>566</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -52628,16 +52621,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>557</v>
+        <v>567</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>559</v>
+        <v>569</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -52645,10 +52638,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>561</v>
+        <v>571</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -52656,10 +52649,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>564</v>
+        <v>574</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -52667,10 +52660,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -52678,10 +52671,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>567</v>
+        <v>577</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>568</v>
+        <v>578</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -52689,10 +52682,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>569</v>
+        <v>579</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -52700,10 +52693,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -52711,10 +52704,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>573</v>
+        <v>583</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>574</v>
+        <v>584</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -52722,10 +52715,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -52733,10 +52726,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>577</v>
+        <v>587</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -52744,10 +52737,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -52755,10 +52748,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -52766,10 +52759,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>97</v>
@@ -52777,10 +52770,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>100</v>
@@ -52788,10 +52781,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>103</v>
@@ -52799,10 +52792,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>589</v>
+        <v>599</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>106</v>
@@ -52810,10 +52803,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>591</v>
+        <v>601</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>592</v>
+        <v>602</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>110</v>
@@ -52821,10 +52814,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>113</v>
@@ -52832,38 +52825,38 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>597</v>
+        <v>607</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>60</v>
@@ -52871,10 +52864,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>64</v>
@@ -52882,10 +52875,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>606</v>
+        <v>616</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>67</v>
@@ -52893,10 +52886,10 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="8" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>608</v>
+        <v>618</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>70</v>
@@ -53916,7 +53909,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>609</v>
+        <v>619</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -53967,16 +53960,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -53984,10 +53977,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="33" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -53995,66 +53988,66 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>618</v>
+        <v>628</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="H6" s="8">
         <v>0.0</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>620</v>
+        <v>630</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>621</v>
+        <v>631</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>623</v>
+        <v>633</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>624</v>
+        <v>634</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="29" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="H7" s="29">
         <v>100.0</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>625</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>627</v>
+        <v>637</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>629</v>
+        <v>639</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
@@ -54062,13 +54055,13 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>631</v>
+        <v>641</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
@@ -54076,13 +54069,13 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>633</v>
+        <v>643</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>67</v>
@@ -54090,19 +54083,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>636</v>
+        <v>646</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -54110,13 +54103,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>639</v>
+        <v>649</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>650</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>640</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>630</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -54124,13 +54117,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>642</v>
+        <v>652</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -54138,13 +54131,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -54152,13 +54145,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>646</v>
+        <v>656</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -54166,13 +54159,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>648</v>
+        <v>658</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -54180,13 +54173,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -55196,8 +55189,7 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -55227,7 +55219,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -55278,16 +55270,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>653</v>
+        <v>663</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -55295,10 +55287,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>655</v>
+        <v>665</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>656</v>
+        <v>666</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -55306,10 +55298,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>657</v>
+        <v>667</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>658</v>
+        <v>668</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -55317,10 +55309,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>659</v>
+        <v>669</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>658</v>
+        <v>668</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
moved 'title' to 'description' field for DCW and LFC atoms
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="884">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -950,8 +950,7 @@
     <t>DCW</t>
   </si>
   <si>
-    <t>Float specifying the density or ratio between the area of columns and/or walls and the area of the building plan.
-(DCW &lt;= 1)</t>
+    <t>Float specifying the density or ratio between the area of columns and/or walls and the area of the building plan.</t>
   </si>
   <si>
     <t>LFM,LFINF,LFBR,LPB,LWAL,LDUAL,LFLS,LFLSINF</t>
@@ -967,6 +966,9 @@
             }</t>
   </si>
   <si>
+    <t>(DCW &lt;= 1)</t>
+  </si>
+  <si>
     <t>height: Height</t>
   </si>
   <si>
@@ -1129,7 +1131,7 @@
     <t>HD</t>
   </si>
   <si>
-    <t>q</t>
+    <t>Slope of the ground (n=float in degrees).</t>
   </si>
   <si>
     <t>HD:n</t>
@@ -4695,7 +4697,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4746,16 +4748,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -4763,10 +4765,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -4774,10 +4776,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -4785,10 +4787,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -4796,10 +4798,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -4807,10 +4809,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -4818,7 +4820,7 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>102</v>
@@ -4829,10 +4831,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -4840,10 +4842,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -4851,10 +4853,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -4862,10 +4864,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -4873,16 +4875,16 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>60</v>
@@ -4890,10 +4892,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>64</v>
@@ -4901,10 +4903,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>67</v>
@@ -4912,10 +4914,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>70</v>
@@ -4923,19 +4925,19 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>60</v>
@@ -4943,13 +4945,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>709</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>710</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>708</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>64</v>
@@ -5978,7 +5980,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6029,16 +6031,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -6046,10 +6048,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -6057,10 +6059,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -6068,10 +6070,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -6079,10 +6081,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -6090,10 +6092,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -6101,10 +6103,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -6112,10 +6114,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -6123,10 +6125,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -6134,10 +6136,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -6145,16 +6147,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>60</v>
@@ -6162,10 +6164,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>64</v>
@@ -6173,10 +6175,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>67</v>
@@ -6184,10 +6186,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>70</v>
@@ -6195,7 +6197,7 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>214</v>
@@ -6206,10 +6208,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>76</v>
@@ -6217,10 +6219,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>79</v>
@@ -6228,10 +6230,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>82</v>
@@ -6239,10 +6241,10 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>85</v>
@@ -6250,10 +6252,10 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>88</v>
@@ -6261,10 +6263,10 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>91</v>
@@ -6272,10 +6274,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>94</v>
@@ -6283,10 +6285,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>97</v>
@@ -6294,16 +6296,16 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>60</v>
@@ -6311,10 +6313,10 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>64</v>
@@ -6322,10 +6324,10 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>67</v>
@@ -6333,10 +6335,10 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>70</v>
@@ -6344,7 +6346,7 @@
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>102</v>
@@ -6355,10 +6357,10 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>76</v>
@@ -6366,10 +6368,10 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>79</v>
@@ -6377,19 +6379,19 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>60</v>
@@ -6397,13 +6399,13 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="8" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>64</v>
@@ -6411,13 +6413,13 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="8" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>67</v>
@@ -6425,13 +6427,13 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="8" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>70</v>
@@ -6439,13 +6441,13 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>73</v>
@@ -6453,13 +6455,13 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>76</v>
@@ -6467,13 +6469,13 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>79</v>
@@ -6481,13 +6483,13 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>82</v>
@@ -6495,13 +6497,13 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>85</v>
@@ -6509,13 +6511,13 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>88</v>
@@ -6523,13 +6525,13 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>91</v>
@@ -6537,13 +6539,13 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="8" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>94</v>
@@ -6551,13 +6553,13 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="8" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>97</v>
@@ -6565,13 +6567,13 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="8" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>100</v>
@@ -6579,13 +6581,13 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>103</v>
@@ -6593,13 +6595,13 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>106</v>
@@ -6607,13 +6609,13 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>110</v>
@@ -6621,13 +6623,13 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>113</v>
@@ -6635,16 +6637,16 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>60</v>
@@ -6652,10 +6654,10 @@
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>64</v>
@@ -6663,10 +6665,10 @@
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>67</v>
@@ -6674,10 +6676,10 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>70</v>
@@ -7675,7 +7677,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7726,16 +7728,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -7743,10 +7745,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -7754,10 +7756,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -7765,10 +7767,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -7776,10 +7778,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -7787,7 +7789,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>102</v>
@@ -7798,10 +7800,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -7809,19 +7811,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -7829,13 +7831,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -7843,13 +7845,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -7857,13 +7859,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -7871,13 +7873,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -7885,13 +7887,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -7899,13 +7901,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -7913,13 +7915,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>82</v>
@@ -7927,13 +7929,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>85</v>
@@ -7941,13 +7943,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>88</v>
@@ -7955,13 +7957,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>91</v>
@@ -7969,13 +7971,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>94</v>
@@ -7983,13 +7985,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>97</v>
@@ -7997,13 +7999,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>100</v>
@@ -8011,16 +8013,16 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>60</v>
@@ -8028,10 +8030,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>64</v>
@@ -9053,7 +9055,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9104,16 +9106,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -9121,10 +9123,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -9132,10 +9134,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -9143,10 +9145,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -9154,10 +9156,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -10193,7 +10195,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10244,16 +10246,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -10261,10 +10263,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -16099,7 +16101,7 @@
     <col customWidth="1" min="2" max="2" width="33.0"/>
     <col customWidth="1" min="3" max="3" width="11.43"/>
     <col customWidth="1" min="4" max="4" width="59.43"/>
-    <col customWidth="1" min="5" max="5" width="16.29"/>
+    <col customWidth="1" min="5" max="5" width="48.29"/>
     <col customWidth="1" min="6" max="6" width="22.71"/>
     <col customWidth="1" min="7" max="7" width="8.43"/>
     <col customWidth="1" min="8" max="8" width="5.0"/>
@@ -16778,10 +16780,12 @@
       <c r="C20" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16" t="s">
@@ -16988,10 +16992,12 @@
       <c r="C26" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="E26" s="20"/>
       <c r="F26" s="22" t="s">
         <v>302</v>
       </c>
@@ -17026,7 +17032,9 @@
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+      <c r="E27" s="21" t="s">
+        <v>304</v>
+      </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
@@ -45310,7 +45318,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -45364,185 +45372,185 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
@@ -49542,7 +49550,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -49593,53 +49601,53 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>67</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
@@ -49647,10 +49655,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
@@ -49658,10 +49666,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>67</v>
@@ -50661,10 +50669,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -50699,7 +50707,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -50750,31 +50758,31 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E4" s="29"/>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -50782,10 +50790,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -50793,10 +50801,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -50804,10 +50812,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -50815,10 +50823,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -50826,10 +50834,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -50837,10 +50845,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -50848,10 +50856,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -50859,10 +50867,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -50870,10 +50878,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -50881,10 +50889,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -50892,25 +50900,25 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="29" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E16" s="29"/>
       <c r="H16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="29" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E17" s="29"/>
       <c r="H17" s="8" t="s">
@@ -50919,10 +50927,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="29" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E18" s="29"/>
       <c r="H18" s="8" t="s">
@@ -50931,10 +50939,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="29" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E19" s="29"/>
       <c r="H19" s="8" t="s">
@@ -50943,10 +50951,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="29" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E20" s="29"/>
       <c r="H20" s="8" t="s">
@@ -50955,10 +50963,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="29" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E21" s="29"/>
       <c r="H21" s="8" t="s">
@@ -50967,640 +50975,640 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="29" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E22" s="29"/>
       <c r="H22" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="29" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E23" s="29"/>
       <c r="H23" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="29" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E24" s="29"/>
       <c r="H24" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="29" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E25" s="29"/>
       <c r="H25" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="29" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E26" s="29"/>
       <c r="H26" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="29" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E27" s="29"/>
       <c r="H27" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="29" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E28" s="29"/>
       <c r="H28" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="29" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E29" s="29"/>
       <c r="H29" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="29" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E30" s="29"/>
       <c r="H30" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E31" s="29"/>
       <c r="H31" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="K31" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="29" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E32" s="29"/>
       <c r="H32" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="29" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E33" s="29"/>
       <c r="H33" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="C34" s="29" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E34" s="29"/>
       <c r="H34" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="K34" s="30"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="29" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E35" s="29"/>
       <c r="H35" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="K35" s="30"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="29" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E36" s="29"/>
       <c r="H36" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K36" s="30"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="29" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E37" s="29"/>
       <c r="H37" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K37" s="30"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E38" s="29"/>
       <c r="H38" s="8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E42" s="29"/>
       <c r="H42" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="K42" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="29" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E45" s="29"/>
       <c r="H45" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="K45" s="30"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="29" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E46" s="29"/>
       <c r="H46" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="K46" s="30"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="29" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E47" s="29"/>
       <c r="H47" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="K47" s="30"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E48" s="29"/>
       <c r="H48" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K48" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="C52" s="8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1">
       <c r="C56" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="C57" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="58" ht="13.5" customHeight="1">
       <c r="C58" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
       <c r="C59" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E59" s="29"/>
       <c r="H59" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="60" ht="13.5" customHeight="1">
       <c r="C60" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="61" ht="13.5" customHeight="1">
       <c r="C61" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="C62" s="8" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="H62" s="8" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="C63" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="64" ht="13.5" customHeight="1">
       <c r="C64" s="8" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="65" ht="13.5" customHeight="1">
       <c r="C65" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="66" ht="13.5" customHeight="1">
       <c r="C66" s="8" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="C67" s="8" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="C68" s="8" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="C69" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="70" ht="13.5" customHeight="1">
       <c r="C70" s="29" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E70" s="29"/>
       <c r="H70" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K70" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="C71" s="29" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E71" s="29"/>
       <c r="H71" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="C72" s="29" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E72" s="29"/>
       <c r="H72" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="C73" s="29" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E73" s="29"/>
       <c r="H73" s="8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="74" ht="13.5" customHeight="1">
       <c r="C74" s="8" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H74" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="75" ht="13.5" customHeight="1"/>
@@ -52570,7 +52578,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -52621,16 +52629,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -52638,10 +52646,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -52649,10 +52657,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -52660,10 +52668,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -52671,10 +52679,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -52682,10 +52690,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -52693,10 +52701,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -52704,10 +52712,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -52715,10 +52723,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -52726,10 +52734,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -52737,10 +52745,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -52748,10 +52756,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -52759,10 +52767,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>97</v>
@@ -52770,10 +52778,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>100</v>
@@ -52781,10 +52789,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>103</v>
@@ -52792,10 +52800,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>106</v>
@@ -52803,10 +52811,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>110</v>
@@ -52814,10 +52822,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>113</v>
@@ -52825,38 +52833,38 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>60</v>
@@ -52864,10 +52872,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>64</v>
@@ -52875,10 +52883,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>67</v>
@@ -52886,10 +52894,10 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="8" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>70</v>
@@ -53909,7 +53917,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -53960,16 +53968,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -53977,10 +53985,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="33" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -53988,66 +53996,66 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="H6" s="8">
         <v>0.0</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="29" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="H7" s="29">
         <v>100.0</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
@@ -54055,13 +54063,13 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>641</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>640</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
@@ -54069,13 +54077,13 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>67</v>
@@ -54083,19 +54091,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -54103,13 +54111,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -54117,13 +54125,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -54131,13 +54139,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -54145,13 +54153,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -54159,13 +54167,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -54173,13 +54181,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -55219,7 +55227,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -55270,16 +55278,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -55287,10 +55295,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -55298,10 +55306,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -55309,10 +55317,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>669</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>668</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
add parameters 'unit_measure' attribute
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="883">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -962,7 +962,8 @@
             "max": 1,
             "max_incl": true,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["ratio", "ratio"]
             }</t>
   </si>
   <si>
@@ -981,7 +982,7 @@
     <t>H</t>
   </si>
   <si>
-    <t>Number of storeys above ground.</t>
+    <t>Number of storeys above ground</t>
   </si>
   <si>
     <t>H:n, exact number of storeys above ground.
@@ -995,14 +996,15 @@
             "min": 0,
             "min_incl": true,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["storey", "storeys"]
 }</t>
   </si>
   <si>
     <t>HAPP</t>
   </si>
   <si>
-    <t>Approximate number of storeys above ground.</t>
+    <t>Approximate number of storeys above ground</t>
   </si>
   <si>
     <t>HAPP:n</t>
@@ -1013,7 +1015,8 @@
             "min": 0,
             "min_incl": true,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["storey", "storeys"]
 }</t>
   </si>
   <si>
@@ -1026,10 +1029,11 @@
     <t>HHT</t>
   </si>
   <si>
-    <t>Total height of the structure, measured from the ground floor. Float specifying the height of the structures in meters. (HHT&gt;= 1)</t>
-  </si>
-  <si>
-    <t>HHT:n</t>
+    <t>Total height of the structure, measured from the ground floor.</t>
+  </si>
+  <si>
+    <t>Total height of the structure, measured from the ground floor. Float specifying the height of the structures in meters. (HHT&gt;= 1)
+HHT:n</t>
   </si>
   <si>
     <t>{
@@ -1037,17 +1041,19 @@
             "min": 1,
             "min_incl": true,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["meter", "meters"]
 }</t>
   </si>
   <si>
     <t>HHI</t>
   </si>
   <si>
-    <t>Inter-storey height (average). Float specifying the average floor height in meters. (HHI&gt;= 1)</t>
-  </si>
-  <si>
-    <t>HHI:n</t>
+    <t>Inter-storey height (average)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Float specifying the average floor height in meters. (HHI&gt;= 1)
+HHI:n</t>
   </si>
   <si>
     <t>number_storeys_below</t>
@@ -1059,10 +1065,8 @@
     <t>HB</t>
   </si>
   <si>
-    <t>Number of storeys below ground (same as number of basements)</t>
-  </si>
-  <si>
-    <t>HB:n, exact number of storeys below ground.
+    <t>Number of storeys below ground (same as number of basements).
+HB:n, exact number of storeys below ground.
 HB:a-b, range of storeys below ground.
 HB:&lt;n, n upper limit of number of storeys below ground (with n excluded).
 HB:&gt;n, n lower limit of number of storeys below ground (with n excluded).</t>
@@ -1100,7 +1104,8 @@
             "min": 0,
             "min_incl": true,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["meter", "meters"]
 }</t>
   </si>
   <si>
@@ -1118,7 +1123,8 @@
             "min": 0,
             "min_incl": true,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["meter", "meters"]
 }</t>
   </si>
   <si>
@@ -1131,10 +1137,11 @@
     <t>HD</t>
   </si>
   <si>
-    <t>Slope of the ground (n=float in degrees).</t>
-  </si>
-  <si>
-    <t>HD:n</t>
+    <t>Slope of the ground</t>
+  </si>
+  <si>
+    <t>Slope of the ground (n=float in degrees).
+HD:n</t>
   </si>
   <si>
     <t>{
@@ -1144,7 +1151,8 @@
             "max": 90,
             "max_incl": false,
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["degree", "degrees"]
 }</t>
   </si>
   <si>
@@ -1172,7 +1180,8 @@
     <t>{
             "type": "rangeable_int",
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["year", "years"]
 }</t>
   </si>
   <si>
@@ -1185,7 +1194,8 @@
     <t>{
             "type": "int",
             "params_min": 1,
-            "params_max": 1
+            "params_max": 1,
+            "unit_measure": ["year", "years"]
 }</t>
   </si>
   <si>
@@ -4697,7 +4707,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4748,16 +4758,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>674</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>675</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -4765,10 +4775,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>676</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>677</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -4776,10 +4786,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>678</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>679</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -4787,10 +4797,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>680</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>681</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -4798,10 +4808,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>682</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>683</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -4809,10 +4819,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>684</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>685</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -4820,7 +4830,7 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>102</v>
@@ -4831,10 +4841,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>687</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>688</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -4842,10 +4852,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>689</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>690</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -4853,10 +4863,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>691</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>692</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -4864,10 +4874,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>693</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>694</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -4875,16 +4885,16 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
+        <v>694</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>695</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="8" t="s">
         <v>696</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>697</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>698</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>60</v>
@@ -4892,10 +4902,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>699</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>700</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>64</v>
@@ -4903,10 +4913,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>701</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>702</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>67</v>
@@ -4914,10 +4924,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>703</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>704</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>70</v>
@@ -4925,19 +4935,19 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
+        <v>704</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>705</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="8" t="s">
         <v>706</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>707</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>708</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>709</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>60</v>
@@ -4945,13 +4955,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
+        <v>709</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>710</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>711</v>
-      </c>
       <c r="F20" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>64</v>
@@ -5980,7 +5990,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6031,16 +6041,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>714</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>715</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>716</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -6048,10 +6058,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>717</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>718</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -6059,10 +6069,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>719</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>720</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -6070,10 +6080,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>721</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>722</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -6081,10 +6091,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>723</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>724</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -6092,10 +6102,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>725</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>726</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -6103,10 +6113,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>727</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>728</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -6114,10 +6124,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>729</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>730</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -6125,10 +6135,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>731</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>732</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -6136,10 +6146,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>733</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>734</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -6147,16 +6157,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>735</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>737</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>738</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>60</v>
@@ -6164,10 +6174,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>739</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>740</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>64</v>
@@ -6175,10 +6185,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>741</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>742</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>67</v>
@@ -6186,10 +6196,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
+        <v>742</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>743</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>744</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>70</v>
@@ -6197,7 +6207,7 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>214</v>
@@ -6208,10 +6218,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
+        <v>745</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>746</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>747</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>76</v>
@@ -6219,10 +6229,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
+        <v>747</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>748</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>749</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>79</v>
@@ -6230,10 +6240,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>750</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>751</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>82</v>
@@ -6241,10 +6251,10 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>85</v>
@@ -6252,10 +6262,10 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>753</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>754</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>88</v>
@@ -6263,10 +6273,10 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>755</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>756</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>91</v>
@@ -6274,10 +6284,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>757</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>758</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>94</v>
@@ -6285,10 +6295,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>759</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>760</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>97</v>
@@ -6296,16 +6306,16 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>761</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="8" t="s">
         <v>762</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>763</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>60</v>
@@ -6313,10 +6323,10 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="8" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>64</v>
@@ -6324,10 +6334,10 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>67</v>
@@ -6335,10 +6345,10 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>766</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>767</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>70</v>
@@ -6346,7 +6356,7 @@
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>102</v>
@@ -6357,10 +6367,10 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="8" t="s">
+        <v>768</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>769</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>770</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>76</v>
@@ -6368,10 +6378,10 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>771</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>772</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>79</v>
@@ -6379,19 +6389,19 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>773</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>774</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>775</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>776</v>
-      </c>
       <c r="F34" s="8" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>60</v>
@@ -6399,13 +6409,13 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>777</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>778</v>
-      </c>
       <c r="F35" s="8" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>64</v>
@@ -6413,13 +6423,13 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="8" t="s">
+        <v>778</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>779</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>780</v>
-      </c>
       <c r="F36" s="8" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>67</v>
@@ -6427,13 +6437,13 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="8" t="s">
+        <v>780</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>781</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>782</v>
-      </c>
       <c r="F37" s="8" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>70</v>
@@ -6441,13 +6451,13 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>783</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>784</v>
-      </c>
       <c r="F38" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>73</v>
@@ -6455,13 +6465,13 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>785</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>786</v>
-      </c>
       <c r="F39" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>76</v>
@@ -6469,13 +6479,13 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>787</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>788</v>
-      </c>
       <c r="F40" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>79</v>
@@ -6483,13 +6493,13 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>789</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>790</v>
-      </c>
       <c r="F41" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>82</v>
@@ -6497,13 +6507,13 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>791</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>792</v>
-      </c>
       <c r="F42" s="8" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>85</v>
@@ -6511,13 +6521,13 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>793</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>794</v>
-      </c>
       <c r="F43" s="8" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>88</v>
@@ -6525,13 +6535,13 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
+        <v>794</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>795</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>796</v>
-      </c>
       <c r="F44" s="8" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>91</v>
@@ -6539,13 +6549,13 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="8" t="s">
+        <v>796</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>797</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>798</v>
-      </c>
       <c r="F45" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>94</v>
@@ -6553,13 +6563,13 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>799</v>
       </c>
-      <c r="D46" s="8" t="s">
-        <v>800</v>
-      </c>
       <c r="F46" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>97</v>
@@ -6567,13 +6577,13 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="8" t="s">
+        <v>800</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>801</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>802</v>
-      </c>
       <c r="F47" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>100</v>
@@ -6581,13 +6591,13 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
+        <v>802</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>803</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>804</v>
-      </c>
       <c r="F48" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>103</v>
@@ -6595,13 +6605,13 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
+        <v>804</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>805</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>806</v>
-      </c>
       <c r="F49" s="8" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>106</v>
@@ -6609,13 +6619,13 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
+        <v>806</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>807</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>808</v>
-      </c>
       <c r="F50" s="8" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>110</v>
@@ -6623,13 +6633,13 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
+        <v>808</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>809</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>810</v>
-      </c>
       <c r="F51" s="8" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>113</v>
@@ -6637,16 +6647,16 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>811</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="8" t="s">
         <v>812</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>813</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>814</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>60</v>
@@ -6654,10 +6664,10 @@
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>815</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>816</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>64</v>
@@ -6665,10 +6675,10 @@
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>817</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>818</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>67</v>
@@ -6676,10 +6686,10 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
+        <v>818</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>819</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>820</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>70</v>
@@ -7677,7 +7687,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7728,16 +7738,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>822</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>823</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>824</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>825</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -7745,10 +7755,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -7756,10 +7766,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -7767,10 +7777,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -7778,10 +7788,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -7789,7 +7799,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>102</v>
@@ -7800,10 +7810,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
+        <v>830</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>831</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>832</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -7811,19 +7821,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>834</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>835</v>
-      </c>
       <c r="D11" s="8" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -7831,13 +7841,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -7845,13 +7855,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
+        <v>836</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>837</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>838</v>
-      </c>
       <c r="F13" s="8" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -7859,13 +7869,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
+        <v>838</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>839</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>840</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -7873,13 +7883,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
+        <v>840</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>841</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>842</v>
-      </c>
       <c r="F15" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -7887,13 +7897,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
+        <v>842</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>843</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>844</v>
-      </c>
       <c r="F16" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -7901,13 +7911,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
+        <v>844</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>845</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>846</v>
-      </c>
       <c r="F17" s="8" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -7915,13 +7925,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>847</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>848</v>
-      </c>
       <c r="F18" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>82</v>
@@ -7929,13 +7939,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
+        <v>848</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>849</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>850</v>
-      </c>
       <c r="F19" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>85</v>
@@ -7943,13 +7953,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>88</v>
@@ -7957,13 +7967,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
+        <v>851</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>852</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>853</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>91</v>
@@ -7971,13 +7981,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
+        <v>853</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>854</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>855</v>
-      </c>
       <c r="F22" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>94</v>
@@ -7985,13 +7995,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
+        <v>855</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>856</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>857</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>97</v>
@@ -7999,13 +8009,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
+        <v>857</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>858</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>859</v>
-      </c>
       <c r="F24" s="8" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>100</v>
@@ -8013,16 +8023,16 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>860</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="8" t="s">
         <v>861</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>862</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>863</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>60</v>
@@ -8030,10 +8040,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
+        <v>863</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>864</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>865</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>64</v>
@@ -9055,7 +9065,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9106,16 +9116,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>867</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>868</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>869</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -9123,10 +9133,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>869</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>870</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>871</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -9134,10 +9144,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
+        <v>871</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>872</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>873</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -9145,10 +9155,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>873</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>874</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>875</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -9156,10 +9166,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
+        <v>875</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>876</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>877</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -10195,7 +10205,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10246,16 +10256,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>879</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>880</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>881</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -10263,10 +10273,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>881</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>882</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>883</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -16107,7 +16117,7 @@
     <col customWidth="1" min="8" max="8" width="5.0"/>
     <col customWidth="1" min="9" max="9" width="5.29"/>
     <col customWidth="1" min="10" max="10" width="51.0"/>
-    <col customWidth="1" min="11" max="11" width="20.86"/>
+    <col customWidth="1" min="11" max="11" width="34.86"/>
     <col customWidth="1" min="12" max="27" width="8.86"/>
   </cols>
   <sheetData>
@@ -45312,7 +45322,7 @@
     <col customWidth="1" min="8" max="8" width="5.0"/>
     <col customWidth="1" min="9" max="9" width="5.29"/>
     <col customWidth="1" min="10" max="10" width="10.29"/>
-    <col customWidth="1" min="11" max="11" width="28.86"/>
+    <col customWidth="1" min="11" max="11" width="38.29"/>
     <col customWidth="1" min="12" max="27" width="8.86"/>
   </cols>
   <sheetData>
@@ -45461,10 +45471,10 @@
         <v>327</v>
       </c>
       <c r="D8" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>328</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>329</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
@@ -45475,13 +45485,13 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>331</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>332</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
@@ -45492,65 +45502,65 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="27" t="s">
         <v>335</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="E10" s="28" t="s">
         <v>336</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>337</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="28" t="s">
         <v>340</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>341</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="27" t="s">
         <v>345</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="28" t="s">
         <v>346</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>347</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
@@ -49544,13 +49554,13 @@
     <col customWidth="1" min="8" max="8" width="5.0"/>
     <col customWidth="1" min="9" max="9" width="5.29"/>
     <col customWidth="1" min="10" max="10" width="13.43"/>
-    <col customWidth="1" min="11" max="11" width="27.29"/>
+    <col customWidth="1" min="11" max="11" width="35.14"/>
     <col customWidth="1" min="12" max="27" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -49601,53 +49611,53 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="29" t="s">
         <v>352</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="E4" s="29" t="s">
         <v>353</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>354</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>356</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="H5" s="29">
+        <v>100.0</v>
+      </c>
+      <c r="K5" s="29" t="s">
         <v>357</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>361</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>362</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
@@ -49655,10 +49665,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>363</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>364</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
@@ -49666,10 +49676,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>365</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>366</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>67</v>
@@ -50707,7 +50717,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -50758,31 +50768,31 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="C4" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="29" t="s">
         <v>370</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>371</v>
       </c>
       <c r="E4" s="29"/>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>373</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>374</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -50790,10 +50800,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -50801,10 +50811,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>377</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>378</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -50812,10 +50822,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -50823,10 +50833,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>381</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>382</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -50834,10 +50844,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>383</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>384</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -50845,10 +50855,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>386</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -50856,10 +50866,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>387</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>388</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -50867,10 +50877,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>390</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -50878,10 +50888,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>392</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -50889,10 +50899,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>393</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>394</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -50900,25 +50910,25 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" s="29" t="s">
         <v>395</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>396</v>
       </c>
       <c r="E16" s="29"/>
       <c r="H16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="D17" s="29" t="s">
         <v>397</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>398</v>
       </c>
       <c r="E17" s="29"/>
       <c r="H17" s="8" t="s">
@@ -50927,10 +50937,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>399</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>400</v>
       </c>
       <c r="E18" s="29"/>
       <c r="H18" s="8" t="s">
@@ -50939,10 +50949,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D19" s="29" t="s">
         <v>401</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>402</v>
       </c>
       <c r="E19" s="29"/>
       <c r="H19" s="8" t="s">
@@ -50951,10 +50961,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="D20" s="29" t="s">
         <v>403</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>404</v>
       </c>
       <c r="E20" s="29"/>
       <c r="H20" s="8" t="s">
@@ -50963,10 +50973,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="D21" s="29" t="s">
         <v>405</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>406</v>
       </c>
       <c r="E21" s="29"/>
       <c r="H21" s="8" t="s">
@@ -50975,640 +50985,640 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="D22" s="29" t="s">
         <v>407</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>408</v>
       </c>
       <c r="E22" s="29"/>
       <c r="H22" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>410</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>411</v>
       </c>
       <c r="E23" s="29"/>
       <c r="H23" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>413</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>414</v>
       </c>
       <c r="E24" s="29"/>
       <c r="H24" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="D25" s="29" t="s">
         <v>416</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>417</v>
       </c>
       <c r="E25" s="29"/>
       <c r="H25" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="D26" s="29" t="s">
         <v>419</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>420</v>
       </c>
       <c r="E26" s="29"/>
       <c r="H26" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="D27" s="29" t="s">
         <v>422</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>423</v>
       </c>
       <c r="E27" s="29"/>
       <c r="H27" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="D28" s="29" t="s">
         <v>425</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>426</v>
       </c>
       <c r="E28" s="29"/>
       <c r="H28" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="D29" s="29" t="s">
         <v>428</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>429</v>
       </c>
       <c r="E29" s="29"/>
       <c r="H29" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="D30" s="29" t="s">
         <v>431</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>432</v>
       </c>
       <c r="E30" s="29"/>
       <c r="H30" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="J30" s="29" t="s">
         <v>433</v>
-      </c>
-      <c r="J30" s="29" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D31" s="29" t="s">
         <v>435</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>436</v>
       </c>
       <c r="E31" s="29"/>
       <c r="H31" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K31" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="D32" s="29" t="s">
         <v>438</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>439</v>
       </c>
       <c r="E32" s="29"/>
       <c r="H32" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="D33" s="29" t="s">
         <v>441</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>442</v>
       </c>
       <c r="E33" s="29"/>
       <c r="H33" s="8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="C34" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="D34" s="29" t="s">
         <v>444</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>445</v>
       </c>
       <c r="E34" s="29"/>
       <c r="H34" s="8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K34" s="30"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>447</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>448</v>
       </c>
       <c r="E35" s="29"/>
       <c r="H35" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K35" s="30"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="D36" s="29" t="s">
         <v>450</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>451</v>
       </c>
       <c r="E36" s="29"/>
       <c r="H36" s="8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K36" s="30"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="D37" s="29" t="s">
         <v>453</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>454</v>
       </c>
       <c r="E37" s="29"/>
       <c r="H37" s="8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K37" s="30"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>456</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>457</v>
       </c>
       <c r="E38" s="29"/>
       <c r="H38" s="8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>460</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="H40" s="8" t="s">
         <v>463</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="H41" s="8" t="s">
         <v>466</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D42" s="29" t="s">
         <v>468</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>469</v>
       </c>
       <c r="E42" s="29"/>
       <c r="H42" s="8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K42" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="H43" s="8" t="s">
         <v>472</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="H44" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="29" t="s">
+        <v>476</v>
+      </c>
+      <c r="D45" s="29" t="s">
         <v>477</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>478</v>
       </c>
       <c r="E45" s="29"/>
       <c r="H45" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K45" s="30"/>
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="D46" s="29" t="s">
         <v>480</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>481</v>
       </c>
       <c r="E46" s="29"/>
       <c r="H46" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K46" s="30"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="D47" s="29" t="s">
         <v>483</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>484</v>
       </c>
       <c r="E47" s="29"/>
       <c r="H47" s="8" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K47" s="30"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D48" s="29" t="s">
         <v>486</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>487</v>
       </c>
       <c r="E48" s="29"/>
       <c r="H48" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K48" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="H49" s="8" t="s">
         <v>490</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="H50" s="8" t="s">
         <v>493</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="H51" s="8" t="s">
         <v>496</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="C52" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="H52" s="8" t="s">
         <v>499</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="H53" s="8" t="s">
         <v>502</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="H54" s="8" t="s">
         <v>505</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="H55" s="8" t="s">
         <v>508</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1">
       <c r="C56" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>510</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="H56" s="8" t="s">
         <v>511</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="C57" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>513</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="H57" s="8" t="s">
         <v>514</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="58" ht="13.5" customHeight="1">
       <c r="C58" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>516</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="H58" s="8" t="s">
         <v>517</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
       <c r="C59" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="D59" s="29" t="s">
         <v>519</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>520</v>
       </c>
       <c r="E59" s="29"/>
       <c r="H59" s="8" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="60" ht="13.5" customHeight="1">
       <c r="C60" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="H60" s="8" t="s">
         <v>523</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="61" ht="13.5" customHeight="1">
       <c r="C61" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="H61" s="8" t="s">
         <v>526</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="C62" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="D62" s="8" t="s">
         <v>528</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="H62" s="8" t="s">
         <v>529</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="C63" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="D63" s="8" t="s">
         <v>531</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="H63" s="8" t="s">
         <v>532</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="64" ht="13.5" customHeight="1">
       <c r="C64" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="D64" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="H64" s="8" t="s">
         <v>535</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="65" ht="13.5" customHeight="1">
       <c r="C65" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="D65" s="8" t="s">
         <v>537</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="H65" s="8" t="s">
         <v>538</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="66" ht="13.5" customHeight="1">
       <c r="C66" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="H66" s="8" t="s">
         <v>541</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="C67" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="H67" s="8" t="s">
         <v>544</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="C68" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="D68" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="H68" s="8" t="s">
         <v>547</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="C69" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="H69" s="8" t="s">
         <v>550</v>
-      </c>
-      <c r="H69" s="8" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="70" ht="13.5" customHeight="1">
       <c r="C70" s="29" t="s">
+        <v>551</v>
+      </c>
+      <c r="D70" s="29" t="s">
         <v>552</v>
-      </c>
-      <c r="D70" s="29" t="s">
-        <v>553</v>
       </c>
       <c r="E70" s="29"/>
       <c r="H70" s="8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K70" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="C71" s="29" t="s">
+        <v>554</v>
+      </c>
+      <c r="D71" s="29" t="s">
         <v>555</v>
-      </c>
-      <c r="D71" s="29" t="s">
-        <v>556</v>
       </c>
       <c r="E71" s="29"/>
       <c r="H71" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="C72" s="29" t="s">
+        <v>557</v>
+      </c>
+      <c r="D72" s="29" t="s">
         <v>558</v>
-      </c>
-      <c r="D72" s="29" t="s">
-        <v>559</v>
       </c>
       <c r="E72" s="29"/>
       <c r="H72" s="8" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="C73" s="29" t="s">
+        <v>560</v>
+      </c>
+      <c r="D73" s="29" t="s">
         <v>561</v>
-      </c>
-      <c r="D73" s="29" t="s">
-        <v>562</v>
       </c>
       <c r="E73" s="29"/>
       <c r="H73" s="8" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="74" ht="13.5" customHeight="1">
       <c r="C74" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="H74" s="8" t="s">
         <v>565</v>
-      </c>
-      <c r="H74" s="8" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="75" ht="13.5" customHeight="1"/>
@@ -52578,7 +52588,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -52629,16 +52639,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>570</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>571</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -52646,10 +52656,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>572</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>573</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -52657,10 +52667,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>574</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>575</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -52668,10 +52678,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>576</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>577</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -52679,10 +52689,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>578</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>579</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -52690,10 +52700,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>580</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>581</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -52701,10 +52711,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>582</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>583</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -52712,10 +52722,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>584</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>585</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -52723,10 +52733,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>586</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>587</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -52734,10 +52744,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>588</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>589</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -52745,10 +52755,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>590</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>591</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -52756,10 +52766,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>592</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>593</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -52767,10 +52777,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>594</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>595</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>97</v>
@@ -52778,10 +52788,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>596</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>597</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>100</v>
@@ -52789,10 +52799,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>598</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>599</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>103</v>
@@ -52800,10 +52810,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>600</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>601</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>106</v>
@@ -52811,10 +52821,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>603</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>110</v>
@@ -52822,10 +52832,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>604</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>605</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>113</v>
@@ -52833,38 +52843,38 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>606</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>607</v>
-      </c>
       <c r="H22" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>609</v>
-      </c>
       <c r="H23" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>612</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>613</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>60</v>
@@ -52872,10 +52882,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>614</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>615</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>64</v>
@@ -52883,10 +52893,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>616</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>617</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>67</v>
@@ -52894,10 +52904,10 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>618</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>619</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>70</v>
@@ -53917,7 +53927,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -53968,16 +53978,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>621</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="33" t="s">
         <v>622</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="D4" s="8" t="s">
         <v>623</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>624</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -53985,10 +53995,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="33" t="s">
+        <v>624</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>625</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>626</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -53996,66 +54006,66 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>630</v>
-      </c>
       <c r="F6" s="29" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H6" s="8">
         <v>0.0</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>632</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>633</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="35" t="s">
         <v>634</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>635</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="29" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H7" s="29">
         <v>100.0</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>637</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>640</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>641</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
@@ -54063,13 +54073,13 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>643</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
@@ -54077,13 +54087,13 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>645</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>67</v>
@@ -54091,19 +54101,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>646</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>649</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -54111,13 +54121,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
+        <v>649</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>651</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -54125,13 +54135,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>652</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>653</v>
-      </c>
       <c r="F13" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -54139,13 +54149,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>655</v>
-      </c>
       <c r="F14" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -54153,13 +54163,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>657</v>
-      </c>
       <c r="F15" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -54167,13 +54177,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>658</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>659</v>
-      </c>
       <c r="F16" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -54181,13 +54191,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>660</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>661</v>
-      </c>
       <c r="F17" s="8" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -55227,7 +55237,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -55278,16 +55288,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>664</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>665</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -55295,10 +55305,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>666</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>667</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -55306,10 +55316,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
+        <v>667</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>668</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>669</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -55317,10 +55327,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
typo fixed for missing LFC parameter description and some new occupancy type
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="835">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -903,6 +903,17 @@
   </si>
   <si>
     <t>LFC:n, n is the lateral force coefficient in percentage (%)</t>
+  </si>
+  <si>
+    <t>{"type": "float",
+            "min": 0.0,
+            "min_incl": true,
+            "max": 100.0,
+            "max_incl": true,
+            "params_min": 1,
+            "params_max": 1,
+            "unit_measure": ["%", "%"]
+            }</t>
   </si>
   <si>
     <t>system_ductility</t>
@@ -1309,6 +1320,12 @@
     <t>Mobile home</t>
   </si>
   <si>
+    <t>RES:6</t>
+  </si>
+  <si>
+    <t>Indigenous housing</t>
+  </si>
+  <si>
     <t>COM</t>
   </si>
   <si>
@@ -1351,79 +1368,52 @@
     <t>Hotels and motels</t>
   </si>
   <si>
-    <t>1800</t>
-  </si>
-  <si>
     <t>COM:4</t>
   </si>
   <si>
     <t>Covered parking garage</t>
   </si>
   <si>
-    <t>1900</t>
-  </si>
-  <si>
     <t>COM:5</t>
   </si>
   <si>
     <t>Entertainment and recreation</t>
   </si>
   <si>
-    <t>2000</t>
-  </si>
-  <si>
     <t>COM:5A</t>
   </si>
   <si>
     <t>Entertainment</t>
   </si>
   <si>
-    <t>2100</t>
-  </si>
-  <si>
     <t>COM:5B</t>
   </si>
   <si>
     <t>Recreation</t>
   </si>
   <si>
-    <t>2200</t>
-  </si>
-  <si>
     <t>COM:5C</t>
   </si>
   <si>
     <t>Religious gathering</t>
   </si>
   <si>
-    <t>2300</t>
-  </si>
-  <si>
     <t>COM:5D</t>
   </si>
   <si>
     <t>Arena</t>
   </si>
   <si>
-    <t>2400</t>
-  </si>
-  <si>
     <t>COM:5E</t>
   </si>
   <si>
     <t>Cinema, auditoriums or concert hall</t>
   </si>
   <si>
-    <t>2500</t>
-  </si>
-  <si>
     <t>MIX</t>
   </si>
   <si>
     <t>Mixed</t>
-  </si>
-  <si>
-    <t>2600</t>
   </si>
   <si>
     <t>{"type": "filtered_atomsgroup('building_occupancy_class', ['MIX'])",
@@ -1438,396 +1428,264 @@
     <t>Industrial</t>
   </si>
   <si>
-    <t>2700</t>
-  </si>
-  <si>
     <t>IND:1</t>
   </si>
   <si>
     <t>Heavy Industry Factories</t>
   </si>
   <si>
-    <t>2800</t>
-  </si>
-  <si>
     <t>IND:2</t>
   </si>
   <si>
     <t>Light Industry Factories</t>
   </si>
   <si>
-    <t>2900</t>
-  </si>
-  <si>
     <t>IND:3</t>
   </si>
   <si>
     <t>Food/Drugs/Chemicals Factories</t>
   </si>
   <si>
-    <t>3000</t>
-  </si>
-  <si>
     <t>IND:4</t>
   </si>
   <si>
     <t>Metals/Minerals Processing Factories</t>
   </si>
   <si>
-    <t>3100</t>
-  </si>
-  <si>
     <t>IND:5</t>
   </si>
   <si>
     <t>High Technology Labs/Factories</t>
   </si>
   <si>
-    <t>3200</t>
-  </si>
-  <si>
     <t>IND:6</t>
   </si>
   <si>
     <t>Construction Offices</t>
   </si>
   <si>
-    <t>3300</t>
-  </si>
-  <si>
     <t>AGR</t>
   </si>
   <si>
     <t>Agriculture</t>
   </si>
   <si>
-    <t>3400</t>
-  </si>
-  <si>
     <t>AGR:1</t>
   </si>
   <si>
     <t>Produce storage</t>
   </si>
   <si>
-    <t>3500</t>
-  </si>
-  <si>
     <t>AGR:2</t>
   </si>
   <si>
     <t>Animal shelter</t>
   </si>
   <si>
-    <t>3600</t>
-  </si>
-  <si>
     <t>AGR:3</t>
   </si>
   <si>
     <t>Agricultural processing</t>
   </si>
   <si>
-    <t>3700</t>
-  </si>
-  <si>
     <t>GOV</t>
   </si>
   <si>
     <t>Government</t>
   </si>
   <si>
-    <t>3800</t>
-  </si>
-  <si>
     <t>GOV:1</t>
   </si>
   <si>
     <t>Government, general services</t>
   </si>
   <si>
-    <t>3900</t>
-  </si>
-  <si>
     <t>GOV:2</t>
   </si>
   <si>
     <t>Government, emergency response</t>
   </si>
   <si>
-    <t>4000</t>
-  </si>
-  <si>
     <t>GOV:2A</t>
   </si>
   <si>
     <t>Government, police station</t>
   </si>
   <si>
-    <t>4100</t>
-  </si>
-  <si>
     <t>GOV:2B</t>
   </si>
   <si>
     <t>Government, fire station</t>
   </si>
   <si>
-    <t>4200</t>
-  </si>
-  <si>
     <t>GOV:2C</t>
   </si>
   <si>
     <t>Government, emergency operation center</t>
   </si>
   <si>
-    <t>4300</t>
-  </si>
-  <si>
     <t>EDU</t>
   </si>
   <si>
     <t>Education</t>
   </si>
   <si>
-    <t>4400</t>
-  </si>
-  <si>
     <t>EDU:1</t>
   </si>
   <si>
     <t>Pre-school facility</t>
   </si>
   <si>
-    <t>4500</t>
-  </si>
-  <si>
     <t>EDU:1A</t>
   </si>
   <si>
     <t>Day care center</t>
   </si>
   <si>
-    <t>4600</t>
-  </si>
-  <si>
     <t>EDU:1B</t>
   </si>
   <si>
     <t>Pre-school / Kindergarten</t>
   </si>
   <si>
-    <t>4700</t>
-  </si>
-  <si>
     <t>EDU:2</t>
   </si>
   <si>
     <t>School</t>
   </si>
   <si>
-    <t>4800</t>
-  </si>
-  <si>
     <t>EDU:2A</t>
   </si>
   <si>
     <t>Elementary/Primary school</t>
   </si>
   <si>
-    <t>4900</t>
-  </si>
-  <si>
     <t>EDU:2B</t>
   </si>
   <si>
     <t>Middle School</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
     <t>EDU:2C</t>
   </si>
   <si>
     <t>High/Secondary School</t>
   </si>
   <si>
-    <t>5100</t>
-  </si>
-  <si>
     <t>EDU:3</t>
   </si>
   <si>
     <t>College/university, offices and/or classrooms</t>
   </si>
   <si>
-    <t>5200</t>
-  </si>
-  <si>
     <t>EDU:4</t>
   </si>
   <si>
     <t>College/university, research facilities and/or labs</t>
   </si>
   <si>
-    <t>5300</t>
-  </si>
-  <si>
     <t>EDU:5</t>
   </si>
   <si>
     <t>Other schools</t>
   </si>
   <si>
-    <t>5400</t>
-  </si>
-  <si>
     <t>HEA</t>
   </si>
   <si>
     <t>Healthcare</t>
   </si>
   <si>
-    <t>5500</t>
-  </si>
-  <si>
     <t>HEA:1</t>
   </si>
   <si>
     <t>Hospital</t>
   </si>
   <si>
-    <t>5600</t>
-  </si>
-  <si>
     <t>HEA:1A</t>
   </si>
   <si>
     <t>Primary Level Hospital</t>
   </si>
   <si>
-    <t>5700</t>
-  </si>
-  <si>
     <t>HEA:B</t>
   </si>
   <si>
     <t>Secondary Level Hospital</t>
   </si>
   <si>
-    <t>5800</t>
-  </si>
-  <si>
     <t>HEA:C</t>
   </si>
   <si>
     <t>Tertiary Level Hospital</t>
   </si>
   <si>
-    <t>5900</t>
-  </si>
-  <si>
     <t>HEA:2</t>
   </si>
   <si>
     <t>Clinic</t>
   </si>
   <si>
-    <t>6000</t>
-  </si>
-  <si>
     <t>HEA:3</t>
   </si>
   <si>
     <t>Basic Health Unit</t>
   </si>
   <si>
-    <t>6100</t>
-  </si>
-  <si>
     <t>HEA:4</t>
   </si>
   <si>
     <t>Specialty Center</t>
   </si>
   <si>
-    <t>6200</t>
-  </si>
-  <si>
     <t>HEA:5</t>
   </si>
   <si>
     <t>Health Post</t>
   </si>
   <si>
-    <t>6300</t>
-  </si>
-  <si>
     <t>HEA:6</t>
   </si>
   <si>
     <t>Rehabilitation Center</t>
   </si>
   <si>
-    <t>6400</t>
-  </si>
-  <si>
     <t>HEA:7</t>
   </si>
   <si>
     <t>Other healthcare facilities</t>
   </si>
   <si>
-    <t>6500</t>
-  </si>
-  <si>
     <t>TRT</t>
   </si>
   <si>
     <t>Transportation</t>
   </si>
   <si>
-    <t>6600</t>
-  </si>
-  <si>
     <t>TRT:1</t>
   </si>
   <si>
     <t>Bus station</t>
   </si>
   <si>
-    <t>6700</t>
-  </si>
-  <si>
     <t>TRT:2</t>
   </si>
   <si>
     <t>Railway station</t>
   </si>
   <si>
-    <t>6800</t>
-  </si>
-  <si>
     <t>TRT:3</t>
   </si>
   <si>
     <t>Airport</t>
   </si>
   <si>
-    <t>6900</t>
-  </si>
-  <si>
     <t>OCO</t>
   </si>
   <si>
     <t>Other occupancy type</t>
   </si>
   <si>
-    <t>7000</t>
-  </si>
-  <si>
     <t>shape: Shape of the Building Plan</t>
   </si>
   <si>
@@ -1951,10 +1809,16 @@
     <t>Y-shape</t>
   </si>
   <si>
+    <t>1800</t>
+  </si>
+  <si>
     <t>PLFI</t>
   </si>
   <si>
     <t>Irregular plan shape</t>
+  </si>
+  <si>
+    <t>1900</t>
   </si>
   <si>
     <t>building_position_within</t>
@@ -4707,7 +4571,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>670</v>
+        <v>622</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4758,16 +4622,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>671</v>
+        <v>623</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>672</v>
+        <v>624</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>673</v>
+        <v>625</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>674</v>
+        <v>626</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -4775,10 +4639,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>675</v>
+        <v>627</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>676</v>
+        <v>628</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -4786,10 +4650,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>677</v>
+        <v>629</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>678</v>
+        <v>630</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -4797,10 +4661,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>679</v>
+        <v>631</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>680</v>
+        <v>632</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -4808,10 +4672,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>681</v>
+        <v>633</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>682</v>
+        <v>634</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -4819,10 +4683,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>683</v>
+        <v>635</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>684</v>
+        <v>636</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -4830,7 +4694,7 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>685</v>
+        <v>637</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>102</v>
@@ -4841,10 +4705,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>686</v>
+        <v>638</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>687</v>
+        <v>639</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -4852,10 +4716,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>688</v>
+        <v>640</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>689</v>
+        <v>641</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -4863,10 +4727,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>690</v>
+        <v>642</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>691</v>
+        <v>643</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -4874,10 +4738,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>692</v>
+        <v>644</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>693</v>
+        <v>645</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -4885,16 +4749,16 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>694</v>
+        <v>646</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>695</v>
+        <v>647</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>696</v>
+        <v>648</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>697</v>
+        <v>649</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>60</v>
@@ -4902,10 +4766,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>698</v>
+        <v>650</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>699</v>
+        <v>651</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>64</v>
@@ -4913,10 +4777,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>700</v>
+        <v>652</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>701</v>
+        <v>653</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>67</v>
@@ -4924,10 +4788,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>702</v>
+        <v>654</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>703</v>
+        <v>655</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>70</v>
@@ -4935,19 +4799,19 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>704</v>
+        <v>656</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>705</v>
+        <v>657</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>706</v>
+        <v>658</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>707</v>
+        <v>659</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>708</v>
+        <v>660</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>60</v>
@@ -4955,13 +4819,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>709</v>
+        <v>661</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>710</v>
+        <v>662</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>708</v>
+        <v>660</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>64</v>
@@ -5990,7 +5854,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>711</v>
+        <v>663</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6041,16 +5905,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>712</v>
+        <v>664</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>713</v>
+        <v>665</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>714</v>
+        <v>666</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>715</v>
+        <v>667</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -6058,10 +5922,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>716</v>
+        <v>668</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>717</v>
+        <v>669</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -6069,10 +5933,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>718</v>
+        <v>670</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>719</v>
+        <v>671</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -6080,10 +5944,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>720</v>
+        <v>672</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>721</v>
+        <v>673</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -6091,10 +5955,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>722</v>
+        <v>674</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>723</v>
+        <v>675</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -6102,10 +5966,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>724</v>
+        <v>676</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>725</v>
+        <v>677</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -6113,10 +5977,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>726</v>
+        <v>678</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>727</v>
+        <v>679</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -6124,10 +5988,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>728</v>
+        <v>680</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>729</v>
+        <v>681</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -6135,10 +5999,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>730</v>
+        <v>682</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>731</v>
+        <v>683</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -6146,10 +6010,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>732</v>
+        <v>684</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>733</v>
+        <v>685</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -6157,16 +6021,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>734</v>
+        <v>686</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>735</v>
+        <v>687</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>736</v>
+        <v>688</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>737</v>
+        <v>689</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>60</v>
@@ -6174,10 +6038,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>738</v>
+        <v>690</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>739</v>
+        <v>691</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>64</v>
@@ -6185,10 +6049,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>740</v>
+        <v>692</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>741</v>
+        <v>693</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>67</v>
@@ -6196,10 +6060,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>742</v>
+        <v>694</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>743</v>
+        <v>695</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>70</v>
@@ -6207,7 +6071,7 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>744</v>
+        <v>696</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>214</v>
@@ -6218,10 +6082,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>745</v>
+        <v>697</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>746</v>
+        <v>698</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>76</v>
@@ -6229,10 +6093,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>747</v>
+        <v>699</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>748</v>
+        <v>700</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>79</v>
@@ -6240,10 +6104,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>749</v>
+        <v>701</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>750</v>
+        <v>702</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>82</v>
@@ -6251,10 +6115,10 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>751</v>
+        <v>703</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>684</v>
+        <v>636</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>85</v>
@@ -6262,10 +6126,10 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>752</v>
+        <v>704</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>753</v>
+        <v>705</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>88</v>
@@ -6273,10 +6137,10 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>754</v>
+        <v>706</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>755</v>
+        <v>707</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>91</v>
@@ -6284,10 +6148,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>756</v>
+        <v>708</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>757</v>
+        <v>709</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>94</v>
@@ -6295,10 +6159,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>758</v>
+        <v>710</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>759</v>
+        <v>711</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>97</v>
@@ -6306,16 +6170,16 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>760</v>
+        <v>712</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>761</v>
+        <v>713</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>762</v>
+        <v>714</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>680</v>
+        <v>632</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>60</v>
@@ -6323,10 +6187,10 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="8" t="s">
-        <v>763</v>
+        <v>715</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>753</v>
+        <v>705</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>64</v>
@@ -6334,10 +6198,10 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="8" t="s">
-        <v>764</v>
+        <v>716</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>674</v>
+        <v>626</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>67</v>
@@ -6345,10 +6209,10 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="8" t="s">
-        <v>765</v>
+        <v>717</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>766</v>
+        <v>718</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>70</v>
@@ -6356,7 +6220,7 @@
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>767</v>
+        <v>719</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>102</v>
@@ -6367,10 +6231,10 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="8" t="s">
-        <v>768</v>
+        <v>720</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>769</v>
+        <v>721</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>76</v>
@@ -6378,10 +6242,10 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="8" t="s">
-        <v>770</v>
+        <v>722</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>771</v>
+        <v>723</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>79</v>
@@ -6389,19 +6253,19 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>772</v>
+        <v>724</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>773</v>
+        <v>725</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>774</v>
+        <v>726</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>775</v>
+        <v>727</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>762</v>
+        <v>714</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>60</v>
@@ -6409,13 +6273,13 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="8" t="s">
-        <v>776</v>
+        <v>728</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>777</v>
+        <v>729</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>762</v>
+        <v>714</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>64</v>
@@ -6423,13 +6287,13 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="8" t="s">
-        <v>778</v>
+        <v>730</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>779</v>
+        <v>731</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>762</v>
+        <v>714</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>67</v>
@@ -6437,13 +6301,13 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="8" t="s">
-        <v>780</v>
+        <v>732</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>781</v>
+        <v>733</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>763</v>
+        <v>715</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>70</v>
@@ -6451,13 +6315,13 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
-        <v>782</v>
+        <v>734</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>783</v>
+        <v>735</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>764</v>
+        <v>716</v>
       </c>
       <c r="H38" s="8" t="s">
         <v>73</v>
@@ -6465,13 +6329,13 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
-        <v>784</v>
+        <v>736</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>785</v>
+        <v>737</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>764</v>
+        <v>716</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>76</v>
@@ -6479,13 +6343,13 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
-        <v>786</v>
+        <v>738</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>787</v>
+        <v>739</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>764</v>
+        <v>716</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>79</v>
@@ -6493,13 +6357,13 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
-        <v>788</v>
+        <v>740</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>789</v>
+        <v>741</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>764</v>
+        <v>716</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>82</v>
@@ -6507,13 +6371,13 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>790</v>
+        <v>742</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>791</v>
+        <v>743</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>765</v>
+        <v>717</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>85</v>
@@ -6521,13 +6385,13 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
-        <v>792</v>
+        <v>744</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>793</v>
+        <v>745</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>765</v>
+        <v>717</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>88</v>
@@ -6535,13 +6399,13 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
-        <v>794</v>
+        <v>746</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>795</v>
+        <v>747</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>765</v>
+        <v>717</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>91</v>
@@ -6549,13 +6413,13 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="8" t="s">
-        <v>796</v>
+        <v>748</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>797</v>
+        <v>749</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>767</v>
+        <v>719</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>94</v>
@@ -6563,13 +6427,13 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="8" t="s">
-        <v>798</v>
+        <v>750</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>799</v>
+        <v>751</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>767</v>
+        <v>719</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>97</v>
@@ -6577,13 +6441,13 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="8" t="s">
-        <v>800</v>
+        <v>752</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>801</v>
+        <v>753</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>767</v>
+        <v>719</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>100</v>
@@ -6591,13 +6455,13 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
-        <v>802</v>
+        <v>754</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>803</v>
+        <v>755</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>767</v>
+        <v>719</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>103</v>
@@ -6605,13 +6469,13 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
-        <v>804</v>
+        <v>756</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>805</v>
+        <v>757</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>767</v>
+        <v>719</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>106</v>
@@ -6619,13 +6483,13 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
-        <v>806</v>
+        <v>758</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>807</v>
+        <v>759</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>768</v>
+        <v>720</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>110</v>
@@ -6633,13 +6497,13 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>808</v>
+        <v>760</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>809</v>
+        <v>761</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>768</v>
+        <v>720</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>113</v>
@@ -6647,16 +6511,16 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>810</v>
+        <v>762</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>811</v>
+        <v>763</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>812</v>
+        <v>764</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>813</v>
+        <v>765</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>60</v>
@@ -6664,10 +6528,10 @@
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>814</v>
+        <v>766</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>815</v>
+        <v>767</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>64</v>
@@ -6675,10 +6539,10 @@
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>816</v>
+        <v>768</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>817</v>
+        <v>769</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>67</v>
@@ -6686,10 +6550,10 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>818</v>
+        <v>770</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>819</v>
+        <v>771</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>70</v>
@@ -7687,7 +7551,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>820</v>
+        <v>772</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7738,16 +7602,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>821</v>
+        <v>773</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>822</v>
+        <v>774</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>823</v>
+        <v>775</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>824</v>
+        <v>776</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -7755,10 +7619,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>825</v>
+        <v>777</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>680</v>
+        <v>632</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -7766,10 +7630,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>826</v>
+        <v>778</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>753</v>
+        <v>705</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -7777,10 +7641,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>827</v>
+        <v>779</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>674</v>
+        <v>626</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -7788,10 +7652,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>828</v>
+        <v>780</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>682</v>
+        <v>634</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -7799,7 +7663,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>829</v>
+        <v>781</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>102</v>
@@ -7810,10 +7674,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>830</v>
+        <v>782</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>831</v>
+        <v>783</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -7821,19 +7685,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>832</v>
+        <v>784</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>833</v>
+        <v>785</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>834</v>
+        <v>786</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>775</v>
+        <v>727</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>825</v>
+        <v>777</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -7841,13 +7705,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>835</v>
+        <v>787</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>777</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>825</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -7855,13 +7719,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>836</v>
+        <v>788</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>837</v>
+        <v>789</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>825</v>
+        <v>777</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -7869,13 +7733,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>838</v>
+        <v>790</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>839</v>
+        <v>791</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>827</v>
+        <v>779</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -7883,13 +7747,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>840</v>
+        <v>792</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>841</v>
+        <v>793</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>827</v>
+        <v>779</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -7897,13 +7761,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>842</v>
+        <v>794</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>843</v>
+        <v>795</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>827</v>
+        <v>779</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -7911,13 +7775,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>844</v>
+        <v>796</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>845</v>
+        <v>797</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>827</v>
+        <v>779</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -7925,13 +7789,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>846</v>
+        <v>798</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>847</v>
+        <v>799</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>828</v>
+        <v>780</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>82</v>
@@ -7939,13 +7803,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>848</v>
+        <v>800</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>849</v>
+        <v>801</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>828</v>
+        <v>780</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>85</v>
@@ -7953,13 +7817,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>850</v>
+        <v>802</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>795</v>
+        <v>747</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>828</v>
+        <v>780</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>88</v>
@@ -7967,13 +7831,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>851</v>
+        <v>803</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>852</v>
+        <v>804</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>829</v>
+        <v>781</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>91</v>
@@ -7981,13 +7845,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>853</v>
+        <v>805</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>854</v>
+        <v>806</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>829</v>
+        <v>781</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>94</v>
@@ -7995,13 +7859,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>855</v>
+        <v>807</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>856</v>
+        <v>808</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>829</v>
+        <v>781</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>97</v>
@@ -8009,13 +7873,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>857</v>
+        <v>809</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>858</v>
+        <v>810</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>829</v>
+        <v>781</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>100</v>
@@ -8023,16 +7887,16 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>859</v>
+        <v>811</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>860</v>
+        <v>812</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>861</v>
+        <v>813</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>862</v>
+        <v>814</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>60</v>
@@ -8040,10 +7904,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>863</v>
+        <v>815</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>864</v>
+        <v>816</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>64</v>
@@ -9065,7 +8929,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>865</v>
+        <v>817</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9116,16 +8980,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>866</v>
+        <v>818</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>867</v>
+        <v>819</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>868</v>
+        <v>820</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -9133,10 +8997,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>869</v>
+        <v>821</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>870</v>
+        <v>822</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -9144,10 +9008,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>871</v>
+        <v>823</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>872</v>
+        <v>824</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -9155,10 +9019,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>873</v>
+        <v>825</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>874</v>
+        <v>826</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -9166,10 +9030,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>875</v>
+        <v>827</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>876</v>
+        <v>828</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -10205,7 +10069,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>877</v>
+        <v>829</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10256,16 +10120,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>878</v>
+        <v>830</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>879</v>
+        <v>831</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>880</v>
+        <v>832</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -10273,10 +10137,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>881</v>
+        <v>833</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>882</v>
+        <v>834</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -16803,7 +16667,9 @@
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="K20" s="21" t="s">
+        <v>286</v>
+      </c>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
@@ -16823,16 +16689,16 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -16862,10 +16728,10 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="16" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
@@ -16895,10 +16761,10 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
@@ -16928,10 +16794,10 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="16" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
@@ -16961,10 +16827,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="16" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
@@ -16994,22 +16860,22 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C26" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>299</v>
-      </c>
       <c r="E26" s="19" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16" t="s">
@@ -17018,7 +16884,7 @@
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="21" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
@@ -17043,7 +16909,7 @@
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
       <c r="E27" s="21" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -45328,7 +45194,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -45382,185 +45248,185 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>327</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>326</v>
-      </c>
       <c r="E8" s="28" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
@@ -49560,7 +49426,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -49611,53 +49477,53 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H5" s="29">
         <v>100.0</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>60</v>
@@ -49665,10 +49531,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>64</v>
@@ -49676,10 +49542,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>67</v>
@@ -50717,7 +50583,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -50768,231 +50634,250 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E4" s="29"/>
       <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>64</v>
+        <v>374</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:H75" si="1">H4+100</f>
+        <v>100</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>67</v>
+        <v>376</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="1"/>
+        <v>200</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>70</v>
+        <v>378</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="1"/>
+        <v>300</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>73</v>
+        <v>380</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="1"/>
+        <v>400</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>76</v>
+        <v>382</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="1"/>
+        <v>500</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>79</v>
+        <v>384</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="1"/>
+        <v>600</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>82</v>
+        <v>386</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="1"/>
+        <v>700</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>85</v>
+        <v>388</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="1"/>
+        <v>800</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>88</v>
+        <v>390</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="1"/>
+        <v>900</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>91</v>
+        <v>392</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="1"/>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>94</v>
+        <v>394</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="1"/>
+        <v>1100</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="29" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E16" s="29"/>
-      <c r="H16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K16" s="29" t="s">
-        <v>371</v>
-      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="29" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E17" s="29"/>
-      <c r="H17" s="8" t="s">
-        <v>100</v>
+      <c r="H17" s="8">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="29" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E18" s="29"/>
-      <c r="H18" s="8" t="s">
-        <v>103</v>
+      <c r="H18" s="8">
+        <f t="shared" si="1"/>
+        <v>1400</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="29" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E19" s="29"/>
-      <c r="H19" s="8" t="s">
-        <v>106</v>
+      <c r="H19" s="8">
+        <f t="shared" si="1"/>
+        <v>1500</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="29" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E20" s="29"/>
-      <c r="H20" s="8" t="s">
-        <v>110</v>
+      <c r="H20" s="8">
+        <f t="shared" si="1"/>
+        <v>1600</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="29" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E21" s="29"/>
-      <c r="H21" s="8" t="s">
-        <v>113</v>
+      <c r="H21" s="8">
+        <f t="shared" si="1"/>
+        <v>1700</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="29" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E22" s="29"/>
-      <c r="H22" s="8" t="s">
-        <v>408</v>
+      <c r="H22" s="8">
+        <f t="shared" si="1"/>
+        <v>1800</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
@@ -51003,625 +50888,689 @@
         <v>410</v>
       </c>
       <c r="E23" s="29"/>
-      <c r="H23" s="8" t="s">
-        <v>411</v>
+      <c r="H23" s="8">
+        <f t="shared" si="1"/>
+        <v>1900</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="29" t="s">
+        <v>411</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>412</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>413</v>
-      </c>
       <c r="E24" s="29"/>
-      <c r="H24" s="8" t="s">
-        <v>414</v>
+      <c r="H24" s="8">
+        <f t="shared" si="1"/>
+        <v>2000</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="29" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E25" s="29"/>
-      <c r="H25" s="8" t="s">
-        <v>417</v>
+      <c r="H25" s="8">
+        <f t="shared" si="1"/>
+        <v>2100</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="29" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E26" s="29"/>
-      <c r="H26" s="8" t="s">
-        <v>420</v>
+      <c r="H26" s="8">
+        <f t="shared" si="1"/>
+        <v>2200</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="29" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E27" s="29"/>
-      <c r="H27" s="8" t="s">
-        <v>423</v>
+      <c r="H27" s="8">
+        <f t="shared" si="1"/>
+        <v>2300</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="29" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E28" s="29"/>
-      <c r="H28" s="8" t="s">
-        <v>426</v>
+      <c r="H28" s="8">
+        <f t="shared" si="1"/>
+        <v>2400</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="29" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="E29" s="29"/>
-      <c r="H29" s="8" t="s">
-        <v>429</v>
+      <c r="H29" s="8">
+        <f t="shared" si="1"/>
+        <v>2500</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E30" s="29"/>
-      <c r="H30" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="J30" s="29" t="s">
-        <v>433</v>
+      <c r="H30" s="8">
+        <f t="shared" si="1"/>
+        <v>2600</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="C31" s="8" t="s">
-        <v>434</v>
+      <c r="C31" s="29" t="s">
+        <v>425</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="E31" s="29"/>
-      <c r="H31" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="K31" s="29" t="s">
-        <v>371</v>
+      <c r="H31" s="8">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+      <c r="J31" s="29" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="C32" s="29" t="s">
-        <v>437</v>
+      <c r="C32" s="8" t="s">
+        <v>428</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="E32" s="29"/>
-      <c r="H32" s="8" t="s">
-        <v>439</v>
+      <c r="H32" s="8">
+        <f t="shared" si="1"/>
+        <v>2800</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="29" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="E33" s="29"/>
-      <c r="H33" s="8" t="s">
-        <v>442</v>
+      <c r="H33" s="8">
+        <f t="shared" si="1"/>
+        <v>2900</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="C34" s="29" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="E34" s="29"/>
-      <c r="H34" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="K34" s="30"/>
+      <c r="H34" s="8">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="29" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="E35" s="29"/>
-      <c r="H35" s="8" t="s">
-        <v>448</v>
+      <c r="H35" s="8">
+        <f t="shared" si="1"/>
+        <v>3100</v>
       </c>
       <c r="K35" s="30"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="29" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="E36" s="29"/>
-      <c r="H36" s="8" t="s">
-        <v>451</v>
+      <c r="H36" s="8">
+        <f t="shared" si="1"/>
+        <v>3200</v>
       </c>
       <c r="K36" s="30"/>
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="29" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="E37" s="29"/>
-      <c r="H37" s="8" t="s">
-        <v>454</v>
+      <c r="H37" s="8">
+        <f t="shared" si="1"/>
+        <v>3300</v>
       </c>
       <c r="K37" s="30"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="C38" s="8" t="s">
-        <v>455</v>
+      <c r="C38" s="29" t="s">
+        <v>440</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="E38" s="29"/>
-      <c r="H38" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="K38" s="29" t="s">
-        <v>371</v>
-      </c>
+      <c r="H38" s="8">
+        <f t="shared" si="1"/>
+        <v>3400</v>
+      </c>
+      <c r="K38" s="30"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>460</v>
+        <v>442</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="H39" s="8">
+        <f t="shared" si="1"/>
+        <v>3500</v>
+      </c>
+      <c r="K39" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>463</v>
+        <v>445</v>
+      </c>
+      <c r="H40" s="8">
+        <f t="shared" si="1"/>
+        <v>3600</v>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>466</v>
+        <v>447</v>
+      </c>
+      <c r="H41" s="8">
+        <f t="shared" si="1"/>
+        <v>3700</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>467</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>468</v>
-      </c>
-      <c r="E42" s="29"/>
-      <c r="H42" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="K42" s="29" t="s">
-        <v>371</v>
+        <v>448</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="H42" s="8">
+        <f t="shared" si="1"/>
+        <v>3800</v>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>472</v>
+        <v>450</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="H43" s="8">
+        <f t="shared" si="1"/>
+        <v>3900</v>
+      </c>
+      <c r="K43" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>475</v>
+        <v>453</v>
+      </c>
+      <c r="H44" s="8">
+        <f t="shared" si="1"/>
+        <v>4000</v>
       </c>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="C45" s="29" t="s">
-        <v>476</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>477</v>
-      </c>
-      <c r="E45" s="29"/>
-      <c r="H45" s="8" t="s">
-        <v>478</v>
-      </c>
-      <c r="K45" s="30"/>
+      <c r="C45" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="1"/>
+        <v>4100</v>
+      </c>
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="29" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="E46" s="29"/>
-      <c r="H46" s="8" t="s">
-        <v>481</v>
+      <c r="H46" s="8">
+        <f t="shared" si="1"/>
+        <v>4200</v>
       </c>
       <c r="K46" s="30"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="29" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="E47" s="29"/>
-      <c r="H47" s="8" t="s">
-        <v>484</v>
+      <c r="H47" s="8">
+        <f t="shared" si="1"/>
+        <v>4300</v>
       </c>
       <c r="K47" s="30"/>
     </row>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="C48" s="8" t="s">
-        <v>485</v>
+      <c r="C48" s="29" t="s">
+        <v>460</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>486</v>
+        <v>461</v>
       </c>
       <c r="E48" s="29"/>
-      <c r="H48" s="8" t="s">
-        <v>487</v>
-      </c>
-      <c r="K48" s="29" t="s">
-        <v>371</v>
-      </c>
+      <c r="H48" s="8">
+        <f t="shared" si="1"/>
+        <v>4400</v>
+      </c>
+      <c r="K48" s="30"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>490</v>
+        <v>462</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="E49" s="29"/>
+      <c r="H49" s="8">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="K49" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
-        <v>491</v>
+        <v>464</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>492</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>493</v>
+        <v>465</v>
+      </c>
+      <c r="H50" s="8">
+        <f t="shared" si="1"/>
+        <v>4600</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>495</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>496</v>
+        <v>467</v>
+      </c>
+      <c r="H51" s="8">
+        <f t="shared" si="1"/>
+        <v>4700</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="C52" s="8" t="s">
-        <v>497</v>
+        <v>468</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>499</v>
+        <v>469</v>
+      </c>
+      <c r="H52" s="8">
+        <f t="shared" si="1"/>
+        <v>4800</v>
       </c>
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>500</v>
+        <v>470</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>502</v>
+        <v>471</v>
+      </c>
+      <c r="H53" s="8">
+        <f t="shared" si="1"/>
+        <v>4900</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>503</v>
+        <v>472</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>505</v>
+        <v>473</v>
+      </c>
+      <c r="H54" s="8">
+        <f t="shared" si="1"/>
+        <v>5000</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>506</v>
+        <v>474</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>508</v>
+        <v>475</v>
+      </c>
+      <c r="H55" s="8">
+        <f t="shared" si="1"/>
+        <v>5100</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1">
       <c r="C56" s="8" t="s">
-        <v>509</v>
+        <v>476</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>511</v>
+        <v>477</v>
+      </c>
+      <c r="H56" s="8">
+        <f t="shared" si="1"/>
+        <v>5200</v>
       </c>
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="C57" s="8" t="s">
-        <v>512</v>
+        <v>478</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>513</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>514</v>
+        <v>479</v>
+      </c>
+      <c r="H57" s="8">
+        <f t="shared" si="1"/>
+        <v>5300</v>
       </c>
     </row>
     <row r="58" ht="13.5" customHeight="1">
       <c r="C58" s="8" t="s">
-        <v>515</v>
+        <v>480</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>517</v>
+        <v>481</v>
+      </c>
+      <c r="H58" s="8">
+        <f t="shared" si="1"/>
+        <v>5400</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1">
       <c r="C59" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>519</v>
-      </c>
-      <c r="E59" s="29"/>
-      <c r="H59" s="8" t="s">
-        <v>520</v>
-      </c>
-      <c r="K59" s="29" t="s">
-        <v>371</v>
+        <v>482</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="H59" s="8">
+        <f t="shared" si="1"/>
+        <v>5500</v>
       </c>
     </row>
     <row r="60" ht="13.5" customHeight="1">
       <c r="C60" s="8" t="s">
-        <v>521</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>522</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>523</v>
+        <v>484</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>485</v>
+      </c>
+      <c r="E60" s="29"/>
+      <c r="H60" s="8">
+        <f t="shared" si="1"/>
+        <v>5600</v>
+      </c>
+      <c r="K60" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="61" ht="13.5" customHeight="1">
       <c r="C61" s="8" t="s">
-        <v>524</v>
+        <v>486</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>525</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>526</v>
+        <v>487</v>
+      </c>
+      <c r="H61" s="8">
+        <f t="shared" si="1"/>
+        <v>5700</v>
       </c>
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="C62" s="8" t="s">
-        <v>527</v>
+        <v>488</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>529</v>
+        <v>489</v>
+      </c>
+      <c r="H62" s="8">
+        <f t="shared" si="1"/>
+        <v>5800</v>
       </c>
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="C63" s="8" t="s">
-        <v>530</v>
+        <v>490</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>532</v>
+        <v>491</v>
+      </c>
+      <c r="H63" s="8">
+        <f t="shared" si="1"/>
+        <v>5900</v>
       </c>
     </row>
     <row r="64" ht="13.5" customHeight="1">
       <c r="C64" s="8" t="s">
-        <v>533</v>
+        <v>492</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>534</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>535</v>
+        <v>493</v>
+      </c>
+      <c r="H64" s="8">
+        <f t="shared" si="1"/>
+        <v>6000</v>
       </c>
     </row>
     <row r="65" ht="13.5" customHeight="1">
       <c r="C65" s="8" t="s">
-        <v>536</v>
+        <v>494</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>537</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>538</v>
+        <v>495</v>
+      </c>
+      <c r="H65" s="8">
+        <f t="shared" si="1"/>
+        <v>6100</v>
       </c>
     </row>
     <row r="66" ht="13.5" customHeight="1">
       <c r="C66" s="8" t="s">
-        <v>539</v>
+        <v>496</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>540</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>541</v>
+        <v>497</v>
+      </c>
+      <c r="H66" s="8">
+        <f t="shared" si="1"/>
+        <v>6200</v>
       </c>
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="C67" s="8" t="s">
-        <v>542</v>
+        <v>498</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>543</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>544</v>
+        <v>499</v>
+      </c>
+      <c r="H67" s="8">
+        <f t="shared" si="1"/>
+        <v>6300</v>
       </c>
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="C68" s="8" t="s">
-        <v>545</v>
+        <v>500</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>547</v>
+        <v>501</v>
+      </c>
+      <c r="H68" s="8">
+        <f t="shared" si="1"/>
+        <v>6400</v>
       </c>
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="C69" s="8" t="s">
-        <v>548</v>
+        <v>502</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>549</v>
-      </c>
-      <c r="H69" s="8" t="s">
-        <v>550</v>
+        <v>503</v>
+      </c>
+      <c r="H69" s="8">
+        <f t="shared" si="1"/>
+        <v>6500</v>
       </c>
     </row>
     <row r="70" ht="13.5" customHeight="1">
-      <c r="C70" s="29" t="s">
-        <v>551</v>
-      </c>
-      <c r="D70" s="29" t="s">
-        <v>552</v>
-      </c>
-      <c r="E70" s="29"/>
-      <c r="H70" s="8" t="s">
-        <v>553</v>
-      </c>
-      <c r="K70" s="29" t="s">
-        <v>371</v>
+      <c r="C70" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="H70" s="8">
+        <f t="shared" si="1"/>
+        <v>6600</v>
       </c>
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="C71" s="29" t="s">
-        <v>554</v>
+        <v>506</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>555</v>
+        <v>507</v>
       </c>
       <c r="E71" s="29"/>
-      <c r="H71" s="8" t="s">
-        <v>556</v>
+      <c r="H71" s="8">
+        <f t="shared" si="1"/>
+        <v>6700</v>
+      </c>
+      <c r="K71" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="C72" s="29" t="s">
-        <v>557</v>
+        <v>508</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>558</v>
+        <v>509</v>
       </c>
       <c r="E72" s="29"/>
-      <c r="H72" s="8" t="s">
-        <v>559</v>
+      <c r="H72" s="8">
+        <f t="shared" si="1"/>
+        <v>6800</v>
       </c>
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="C73" s="29" t="s">
-        <v>560</v>
+        <v>510</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>561</v>
+        <v>511</v>
       </c>
       <c r="E73" s="29"/>
-      <c r="H73" s="8" t="s">
-        <v>562</v>
+      <c r="H73" s="8">
+        <f t="shared" si="1"/>
+        <v>6900</v>
       </c>
     </row>
     <row r="74" ht="13.5" customHeight="1">
-      <c r="C74" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>564</v>
-      </c>
-      <c r="H74" s="8" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="75" ht="13.5" customHeight="1"/>
+      <c r="C74" s="29" t="s">
+        <v>512</v>
+      </c>
+      <c r="D74" s="29" t="s">
+        <v>513</v>
+      </c>
+      <c r="E74" s="29"/>
+      <c r="H74" s="8">
+        <f t="shared" si="1"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="75" ht="13.5" customHeight="1">
+      <c r="C75" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="H75" s="8">
+        <f t="shared" si="1"/>
+        <v>7100</v>
+      </c>
+    </row>
     <row r="76" ht="13.5" customHeight="1"/>
     <row r="77" ht="13.5" customHeight="1"/>
     <row r="78" ht="13.5" customHeight="1"/>
@@ -52549,11 +52498,12 @@
     <row r="1000" ht="13.5" customHeight="1"/>
     <row r="1001" ht="13.5" customHeight="1"/>
     <row r="1002" ht="13.5" customHeight="1"/>
+    <row r="1003" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A4:A74"/>
-    <mergeCell ref="B4:B74"/>
+    <mergeCell ref="A4:A75"/>
+    <mergeCell ref="B4:B75"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -52588,7 +52538,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>566</v>
+        <v>516</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -52639,16 +52589,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>567</v>
+        <v>517</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>568</v>
+        <v>518</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>569</v>
+        <v>519</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>570</v>
+        <v>520</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -52656,10 +52606,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>571</v>
+        <v>521</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>572</v>
+        <v>522</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -52667,10 +52617,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>573</v>
+        <v>523</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>574</v>
+        <v>524</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -52678,10 +52628,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>575</v>
+        <v>525</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>576</v>
+        <v>526</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -52689,10 +52639,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>577</v>
+        <v>527</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>578</v>
+        <v>528</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -52700,10 +52650,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>579</v>
+        <v>529</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>580</v>
+        <v>530</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -52711,10 +52661,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>581</v>
+        <v>531</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>582</v>
+        <v>532</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -52722,10 +52672,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>583</v>
+        <v>533</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>584</v>
+        <v>534</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -52733,10 +52683,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>585</v>
+        <v>535</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>586</v>
+        <v>536</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -52744,10 +52694,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>587</v>
+        <v>537</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>588</v>
+        <v>538</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -52755,10 +52705,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>589</v>
+        <v>539</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>590</v>
+        <v>540</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -52766,10 +52716,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>591</v>
+        <v>541</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>592</v>
+        <v>542</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -52777,10 +52727,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>593</v>
+        <v>543</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>594</v>
+        <v>544</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>97</v>
@@ -52788,10 +52738,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>595</v>
+        <v>545</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>596</v>
+        <v>546</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>100</v>
@@ -52799,10 +52749,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>597</v>
+        <v>547</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>598</v>
+        <v>548</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>103</v>
@@ -52810,10 +52760,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>599</v>
+        <v>549</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>106</v>
@@ -52821,10 +52771,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>601</v>
+        <v>551</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>602</v>
+        <v>552</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>110</v>
@@ -52832,10 +52782,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>603</v>
+        <v>553</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>604</v>
+        <v>554</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>113</v>
@@ -52843,38 +52793,38 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>605</v>
+        <v>555</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>606</v>
+        <v>556</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>408</v>
+        <v>557</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>607</v>
+        <v>558</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>608</v>
+        <v>559</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>411</v>
+        <v>560</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>609</v>
+        <v>561</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>610</v>
+        <v>562</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>611</v>
+        <v>563</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>612</v>
+        <v>564</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>60</v>
@@ -52882,10 +52832,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>613</v>
+        <v>565</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>614</v>
+        <v>566</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>64</v>
@@ -52893,10 +52843,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>615</v>
+        <v>567</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>616</v>
+        <v>568</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>67</v>
@@ -52904,10 +52854,10 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="8" t="s">
-        <v>617</v>
+        <v>569</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>618</v>
+        <v>570</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>70</v>
@@ -53927,7 +53877,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>619</v>
+        <v>571</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -53978,16 +53928,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>620</v>
+        <v>572</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>621</v>
+        <v>573</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>622</v>
+        <v>574</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>623</v>
+        <v>575</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -53995,10 +53945,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="33" t="s">
-        <v>624</v>
+        <v>576</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>625</v>
+        <v>577</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -54006,66 +53956,66 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>626</v>
+        <v>578</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>627</v>
+        <v>579</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>628</v>
+        <v>580</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>629</v>
+        <v>581</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>624</v>
+        <v>576</v>
       </c>
       <c r="H6" s="8">
         <v>0.0</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>630</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>631</v>
+        <v>583</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>632</v>
+        <v>584</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>633</v>
+        <v>585</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>634</v>
+        <v>586</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="29" t="s">
-        <v>624</v>
+        <v>576</v>
       </c>
       <c r="H7" s="29">
         <v>100.0</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>635</v>
+        <v>587</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>636</v>
+        <v>588</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>637</v>
+        <v>589</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>638</v>
+        <v>590</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>639</v>
+        <v>591</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
@@ -54073,13 +54023,13 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>641</v>
+        <v>593</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>642</v>
+        <v>594</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
@@ -54087,13 +54037,13 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>643</v>
+        <v>595</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>644</v>
+        <v>596</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>67</v>
@@ -54101,19 +54051,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>645</v>
+        <v>597</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>646</v>
+        <v>598</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>647</v>
+        <v>599</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>648</v>
+        <v>600</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -54121,13 +54071,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>649</v>
+        <v>601</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>650</v>
+        <v>602</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -54135,13 +54085,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>651</v>
+        <v>603</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>652</v>
+        <v>604</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -54149,13 +54099,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>653</v>
+        <v>605</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>654</v>
+        <v>606</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -54163,13 +54113,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>655</v>
+        <v>607</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>656</v>
+        <v>608</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -54177,13 +54127,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>657</v>
+        <v>609</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>658</v>
+        <v>610</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -54191,13 +54141,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>659</v>
+        <v>611</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>660</v>
+        <v>612</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>640</v>
+        <v>592</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -55237,7 +55187,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>661</v>
+        <v>613</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -55288,16 +55238,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>662</v>
+        <v>614</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>663</v>
+        <v>615</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>664</v>
+        <v>616</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -55305,10 +55255,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>665</v>
+        <v>617</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>666</v>
+        <v>618</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -55316,10 +55266,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>667</v>
+        <v>619</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>668</v>
+        <v>620</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -55327,10 +55277,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>669</v>
+        <v>621</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>668</v>
+        <v>620</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
rearrange roof_system_material and roof_system_type into a single roof_type with parameters
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -23,8 +23,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A27">
+      <text>
+        <t xml:space="preserve">@catalina.yepes@globalquakemodel.org  my proposal is merge material and type together using the same approach used for occupancy:
+material =&gt; ATOM
+type =&gt; Parameter
+	-Matteo Nastasi</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="833">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -2280,154 +2298,148 @@
     <t>Roof covering, other</t>
   </si>
   <si>
-    <t>roof_system_material</t>
-  </si>
-  <si>
-    <t>Roof system material</t>
+    <t>roof_type</t>
+  </si>
+  <si>
+    <t>Roof type</t>
   </si>
   <si>
     <t>RM</t>
   </si>
   <si>
+    <t>RM:1</t>
+  </si>
+  <si>
+    <t>Vaulted masonry</t>
+  </si>
+  <si>
+    <t>RM:2</t>
+  </si>
+  <si>
+    <t>Shallow-arched masonry</t>
+  </si>
+  <si>
+    <t>RM:3</t>
+  </si>
+  <si>
+    <t>Composite masonry and concrete roof system</t>
+  </si>
+  <si>
     <t>RE</t>
   </si>
   <si>
+    <t>RE:1</t>
+  </si>
+  <si>
+    <t>Vaulted earthen roof</t>
+  </si>
+  <si>
     <t>RC</t>
   </si>
   <si>
+    <t>RC:1</t>
+  </si>
+  <si>
+    <t>Cast-in-place beamless reinforced concrete roof</t>
+  </si>
+  <si>
+    <t>RC:2</t>
+  </si>
+  <si>
+    <t>Cast-in-place  beam-supported reinforced concrete roof</t>
+  </si>
+  <si>
+    <t>RC:3</t>
+  </si>
+  <si>
+    <t>Precast concrete roof with reinforced concrete topping</t>
+  </si>
+  <si>
+    <t>RC:4</t>
+  </si>
+  <si>
+    <t>Precast concrete roof without reinforced concrete topping</t>
+  </si>
+  <si>
     <t>RME</t>
   </si>
   <si>
     <t>Metal or steel</t>
   </si>
   <si>
+    <t>RME:1</t>
+  </si>
+  <si>
+    <t>Metal or steel beams or trusses supporting light roofing</t>
+  </si>
+  <si>
+    <t>RME:2</t>
+  </si>
+  <si>
+    <t>Metal or steel beams supporting precast concrete slabs</t>
+  </si>
+  <si>
+    <t>RME:3</t>
+  </si>
+  <si>
+    <t>Composite steel deck and concrete slab</t>
+  </si>
+  <si>
     <t>RWO</t>
   </si>
   <si>
+    <t>RWO:1</t>
+  </si>
+  <si>
+    <t>Wooden structurewith light roof covering</t>
+  </si>
+  <si>
+    <t>RWO:2</t>
+  </si>
+  <si>
+    <t>Wooden beams or trusses with  heavy roof covering</t>
+  </si>
+  <si>
+    <t>RWO:3</t>
+  </si>
+  <si>
+    <t>Wood-based sheets on rafters or purlins</t>
+  </si>
+  <si>
+    <t>RWO:4</t>
+  </si>
+  <si>
+    <t>Plywood panels or other light-weight panels for roof</t>
+  </si>
+  <si>
+    <t>RWO:5</t>
+  </si>
+  <si>
+    <t>Bamboo, straw or thatch roof</t>
+  </si>
+  <si>
     <t>RFA</t>
   </si>
   <si>
     <t>Fabric</t>
   </si>
   <si>
+    <t>RFA:1</t>
+  </si>
+  <si>
+    <t>Inflatable or tensile membrane roof</t>
+  </si>
+  <si>
+    <t>RFA:O</t>
+  </si>
+  <si>
+    <t>Fabric, other</t>
+  </si>
+  <si>
     <t>RO</t>
   </si>
   <si>
     <t>Roof material, other</t>
-  </si>
-  <si>
-    <t>roof_system_type</t>
-  </si>
-  <si>
-    <t>Roof system type</t>
-  </si>
-  <si>
-    <t>RM1</t>
-  </si>
-  <si>
-    <t>Vaulted masonry</t>
-  </si>
-  <si>
-    <t>RM2</t>
-  </si>
-  <si>
-    <t>Shallow-arched masonry</t>
-  </si>
-  <si>
-    <t>RM3</t>
-  </si>
-  <si>
-    <t>Composite masonry and concrete roof system</t>
-  </si>
-  <si>
-    <t>RE1</t>
-  </si>
-  <si>
-    <t>Vaulted earthen roof</t>
-  </si>
-  <si>
-    <t>RC1</t>
-  </si>
-  <si>
-    <t>Cast-in-place beamless reinforced concrete roof</t>
-  </si>
-  <si>
-    <t>RC2</t>
-  </si>
-  <si>
-    <t>Cast-in-place  beam-supported reinforced concrete roof</t>
-  </si>
-  <si>
-    <t>RC3</t>
-  </si>
-  <si>
-    <t>Precast concrete roof with reinforced concrete topping</t>
-  </si>
-  <si>
-    <t>RC4</t>
-  </si>
-  <si>
-    <t>Precast concrete roof without reinforced concrete topping</t>
-  </si>
-  <si>
-    <t>RME1</t>
-  </si>
-  <si>
-    <t>Metal or steel beams or trusses supporting light roofing</t>
-  </si>
-  <si>
-    <t>RME2</t>
-  </si>
-  <si>
-    <t>Metal or steel beams supporting precast concrete slabs</t>
-  </si>
-  <si>
-    <t>RME3</t>
-  </si>
-  <si>
-    <t>Composite steel deck and concrete slab</t>
-  </si>
-  <si>
-    <t>RWO1</t>
-  </si>
-  <si>
-    <t>Wooden structurewith light roof covering</t>
-  </si>
-  <si>
-    <t>RWO2</t>
-  </si>
-  <si>
-    <t>Wooden beams or trusses with  heavy roof covering</t>
-  </si>
-  <si>
-    <t>RWO3</t>
-  </si>
-  <si>
-    <t>Wood-based sheets on rafters or purlins</t>
-  </si>
-  <si>
-    <t>RWO4</t>
-  </si>
-  <si>
-    <t>Plywood panels or other light-weight panels for roof</t>
-  </si>
-  <si>
-    <t>RWO5</t>
-  </si>
-  <si>
-    <t>Bamboo, straw or thatch roof</t>
-  </si>
-  <si>
-    <t>RFA1</t>
-  </si>
-  <si>
-    <t>Inflatable or tensile membrane roof</t>
-  </si>
-  <si>
-    <t>RFAO</t>
-  </si>
-  <si>
-    <t>Fabric, other</t>
   </si>
   <si>
     <t>roof_connections</t>
@@ -2747,7 +2759,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2849,6 +2861,10 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3469,78 +3485,73 @@
     <row r="42" ht="13.5" customHeight="1">
       <c r="D42" s="8" t="str">
         <f>roof!B27</f>
-        <v>Roof system material</v>
+        <v>Roof type</v>
       </c>
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="D43" s="8" t="str">
-        <f>roof!B34</f>
-        <v>Roof system type</v>
-      </c>
-    </row>
-    <row r="44" ht="13.5" customHeight="1">
-      <c r="D44" s="8" t="str">
         <f>roof!B52</f>
         <v>Roof connections</v>
       </c>
     </row>
-    <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="6" t="s">
+    <row r="44" ht="13.5" customHeight="1">
+      <c r="A44" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="8" t="str">
+      <c r="D44" s="8" t="str">
         <f>floor!B4</f>
         <v>Floor system material</v>
       </c>
     </row>
+    <row r="45" ht="13.5" customHeight="1">
+      <c r="D45" s="8" t="str">
+        <f>floor!B11</f>
+        <v>Floor system type</v>
+      </c>
+    </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="D46" s="8" t="str">
-        <f>floor!B11</f>
-        <v>Floor system type</v>
-      </c>
-    </row>
-    <row r="47" ht="13.5" customHeight="1">
-      <c r="D47" s="8" t="str">
         <f>floor!B25</f>
         <v>Floor connections</v>
       </c>
     </row>
+    <row r="47" ht="13.5" customHeight="1">
+      <c r="A47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="8" t="str">
+        <f>foundation!B4</f>
+        <v>Foundation System</v>
+      </c>
+    </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D48" s="8" t="str">
-        <f>foundation!B4</f>
-        <v>Foundation System</v>
-      </c>
-    </row>
-    <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="8" t="str">
         <f>fire_prot!B4</f>
         <v>Fire protection</v>
       </c>
     </row>
+    <row r="49" ht="13.5" customHeight="1"/>
     <row r="50" ht="13.5" customHeight="1"/>
     <row r="51" ht="13.5" customHeight="1"/>
     <row r="52" ht="13.5" customHeight="1"/>
@@ -4491,7 +4502,6 @@
     <row r="997" ht="13.5" customHeight="1"/>
     <row r="998" ht="13.5" customHeight="1"/>
     <row r="999" ht="13.5" customHeight="1"/>
-    <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
     <mergeCell ref="A1:D1"/>
@@ -4510,18 +4520,18 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="C40:C44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="C31:C35"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="C37:C39"/>
-    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A40:A43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink display="material sheet" location="material!A1" ref="C4"/>
@@ -4534,9 +4544,9 @@
     <hyperlink display="hydrodynamics sheet" location="hydrodynamics!A1" ref="C36"/>
     <hyperlink display="ext_walls sheet" location="ext_walls!A1" ref="C37"/>
     <hyperlink display="roof sheet" location="roof!A1" ref="C40"/>
-    <hyperlink display="floor sheet" location="floor!A1" ref="C45"/>
-    <hyperlink display="foundation sheet" location="foundation!A1" ref="C48"/>
-    <hyperlink display="fire_prot sheet" location="fire_prot!A1" ref="C49"/>
+    <hyperlink display="floor sheet" location="floor!A1" ref="C44"/>
+    <hyperlink display="foundation sheet" location="foundation!A1" ref="C47"/>
+    <hyperlink display="fire_prot sheet" location="fire_prot!A1" ref="C48"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -5848,7 +5858,7 @@
     <col customWidth="1" min="8" max="8" width="5.0"/>
     <col customWidth="1" min="9" max="9" width="5.29"/>
     <col customWidth="1" min="10" max="10" width="10.29"/>
-    <col customWidth="1" min="11" max="11" width="10.71"/>
+    <col customWidth="1" min="11" max="11" width="17.0"/>
     <col customWidth="1" min="12" max="27" width="8.86"/>
   </cols>
   <sheetData>
@@ -5916,8 +5926,8 @@
       <c r="D4" s="8" t="s">
         <v>667</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>60</v>
+      <c r="H4" s="36">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
@@ -5927,8 +5937,8 @@
       <c r="D5" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>64</v>
+      <c r="H5" s="36">
+        <v>100.0</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
@@ -5938,8 +5948,8 @@
       <c r="D6" s="8" t="s">
         <v>671</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>67</v>
+      <c r="H6" s="36">
+        <v>200.0</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
@@ -5949,8 +5959,8 @@
       <c r="D7" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>70</v>
+      <c r="H7" s="36">
+        <v>300.0</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
@@ -5960,8 +5970,8 @@
       <c r="D8" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>73</v>
+      <c r="H8" s="36">
+        <v>400.0</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
@@ -5971,8 +5981,8 @@
       <c r="D9" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>76</v>
+      <c r="H9" s="36">
+        <v>500.0</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
@@ -5982,8 +5992,8 @@
       <c r="D10" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>79</v>
+      <c r="H10" s="36">
+        <v>600.0</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
@@ -5993,8 +6003,8 @@
       <c r="D11" s="8" t="s">
         <v>681</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>82</v>
+      <c r="H11" s="36">
+        <v>700.0</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
@@ -6004,8 +6014,8 @@
       <c r="D12" s="8" t="s">
         <v>683</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>85</v>
+      <c r="H12" s="36">
+        <v>800.0</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
@@ -6015,8 +6025,8 @@
       <c r="D13" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>88</v>
+      <c r="H13" s="36">
+        <v>900.0</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
@@ -6032,8 +6042,8 @@
       <c r="D14" s="8" t="s">
         <v>689</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>60</v>
+      <c r="H14" s="36">
+        <v>0.0</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
@@ -6043,8 +6053,8 @@
       <c r="D15" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>64</v>
+      <c r="H15" s="36">
+        <v>100.0</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
@@ -6054,8 +6064,8 @@
       <c r="D16" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>67</v>
+      <c r="H16" s="36">
+        <v>200.0</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
@@ -6065,8 +6075,8 @@
       <c r="D17" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>70</v>
+      <c r="H17" s="36">
+        <v>300.0</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1">
@@ -6076,8 +6086,8 @@
       <c r="D18" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>73</v>
+      <c r="H18" s="36">
+        <v>400.0</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1">
@@ -6087,8 +6097,8 @@
       <c r="D19" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>76</v>
+      <c r="H19" s="36">
+        <v>500.0</v>
       </c>
     </row>
     <row r="20" ht="13.5" customHeight="1">
@@ -6098,8 +6108,8 @@
       <c r="D20" s="8" t="s">
         <v>700</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>79</v>
+      <c r="H20" s="36">
+        <v>600.0</v>
       </c>
     </row>
     <row r="21" ht="13.5" customHeight="1">
@@ -6109,8 +6119,8 @@
       <c r="D21" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>82</v>
+      <c r="H21" s="36">
+        <v>700.0</v>
       </c>
     </row>
     <row r="22" ht="13.5" customHeight="1">
@@ -6120,8 +6130,8 @@
       <c r="D22" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>85</v>
+      <c r="H22" s="36">
+        <v>800.0</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
@@ -6131,8 +6141,8 @@
       <c r="D23" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="H23" s="8" t="s">
-        <v>88</v>
+      <c r="H23" s="36">
+        <v>900.0</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
@@ -6142,8 +6152,8 @@
       <c r="D24" s="8" t="s">
         <v>707</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>91</v>
+      <c r="H24" s="36">
+        <v>1000.0</v>
       </c>
     </row>
     <row r="25" ht="13.5" customHeight="1">
@@ -6153,8 +6163,8 @@
       <c r="D25" s="8" t="s">
         <v>709</v>
       </c>
-      <c r="H25" s="8" t="s">
-        <v>94</v>
+      <c r="H25" s="36">
+        <v>1100.0</v>
       </c>
     </row>
     <row r="26" ht="13.5" customHeight="1">
@@ -6164,15 +6174,15 @@
       <c r="D26" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="H26" s="8" t="s">
-        <v>97</v>
+      <c r="H26" s="36">
+        <v>1200.0</v>
       </c>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="32" t="s">
         <v>712</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="32" t="s">
         <v>713</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -6181,382 +6191,343 @@
       <c r="D27" s="8" t="s">
         <v>632</v>
       </c>
-      <c r="H27" s="8" t="s">
-        <v>60</v>
+      <c r="H27" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="29" t="s">
         <v>715</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>705</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>64</v>
+        <v>716</v>
+      </c>
+      <c r="H28" s="37">
+        <v>100.0</v>
       </c>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="C29" s="8" t="s">
-        <v>716</v>
+      <c r="C29" s="29" t="s">
+        <v>717</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>626</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>67</v>
+        <v>718</v>
+      </c>
+      <c r="H29" s="36">
+        <v>200.0</v>
       </c>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="C30" s="8" t="s">
-        <v>717</v>
+      <c r="C30" s="29" t="s">
+        <v>719</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>718</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>70</v>
+        <v>720</v>
+      </c>
+      <c r="H30" s="37">
+        <v>300.0</v>
       </c>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>73</v>
+        <v>705</v>
+      </c>
+      <c r="H31" s="36">
+        <v>400.0</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="C32" s="8" t="s">
-        <v>720</v>
+      <c r="C32" s="29" t="s">
+        <v>722</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>721</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>76</v>
+        <v>723</v>
+      </c>
+      <c r="H32" s="37">
+        <v>500.0</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="8" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>723</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>79</v>
+        <v>626</v>
+      </c>
+      <c r="H33" s="36">
+        <v>600.0</v>
+      </c>
+      <c r="K33" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="6" t="s">
-        <v>724</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="C34" s="29" t="s">
         <v>725</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>726</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="H34" s="37">
+        <v>700.0</v>
+      </c>
+    </row>
+    <row r="35" ht="13.5" customHeight="1">
+      <c r="C35" s="29" t="s">
         <v>727</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>714</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" ht="13.5" customHeight="1">
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="H35" s="36">
+        <v>800.0</v>
+      </c>
+    </row>
+    <row r="36" ht="13.5" customHeight="1">
+      <c r="C36" s="29" t="s">
         <v>729</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>714</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" ht="13.5" customHeight="1">
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="H36" s="37">
+        <v>900.0</v>
+      </c>
+    </row>
+    <row r="37" ht="13.5" customHeight="1">
+      <c r="C37" s="29" t="s">
         <v>731</v>
       </c>
-      <c r="F36" s="8" t="s">
-        <v>714</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" ht="13.5" customHeight="1">
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>732</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>715</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>70</v>
+      <c r="H37" s="36">
+        <v>1000.0</v>
       </c>
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="H38" s="37">
+        <v>1100.0</v>
+      </c>
+      <c r="K38" s="29" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="39" ht="13.5" customHeight="1">
+      <c r="C39" s="29" t="s">
         <v>735</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" ht="13.5" customHeight="1">
-      <c r="C39" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="H39" s="36">
+        <v>1200.0</v>
+      </c>
+    </row>
+    <row r="40" ht="13.5" customHeight="1">
+      <c r="C40" s="29" t="s">
         <v>737</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" ht="13.5" customHeight="1">
-      <c r="C40" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>738</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="H40" s="37">
+        <v>1300.0</v>
+      </c>
+    </row>
+    <row r="41" ht="13.5" customHeight="1">
+      <c r="C41" s="29" t="s">
         <v>739</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" ht="13.5" customHeight="1">
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>741</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>82</v>
+      <c r="H41" s="36">
+        <v>1400.0</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H42" s="37">
+        <v>1500.0</v>
+      </c>
+      <c r="K42" s="29" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" ht="13.5" customHeight="1">
+      <c r="C43" s="29" t="s">
         <v>742</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D43" s="8" t="s">
         <v>743</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>717</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" ht="13.5" customHeight="1">
-      <c r="C43" s="8" t="s">
+      <c r="H43" s="36">
+        <v>1600.0</v>
+      </c>
+    </row>
+    <row r="44" ht="13.5" customHeight="1">
+      <c r="C44" s="29" t="s">
         <v>744</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>745</v>
       </c>
-      <c r="F43" s="8" t="s">
-        <v>717</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" ht="13.5" customHeight="1">
-      <c r="C44" s="8" t="s">
+      <c r="H44" s="37">
+        <v>1700.0</v>
+      </c>
+    </row>
+    <row r="45" ht="13.5" customHeight="1">
+      <c r="C45" s="29" t="s">
         <v>746</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D45" s="8" t="s">
         <v>747</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>717</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" ht="13.5" customHeight="1">
-      <c r="C45" s="8" t="s">
+      <c r="H45" s="36">
+        <v>1800.0</v>
+      </c>
+    </row>
+    <row r="46" ht="13.5" customHeight="1">
+      <c r="C46" s="29" t="s">
         <v>748</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D46" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" ht="13.5" customHeight="1">
-      <c r="C46" s="8" t="s">
+      <c r="H46" s="37">
+        <v>1900.0</v>
+      </c>
+    </row>
+    <row r="47" ht="13.5" customHeight="1">
+      <c r="C47" s="29" t="s">
         <v>750</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>751</v>
       </c>
-      <c r="F46" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" ht="13.5" customHeight="1">
-      <c r="C47" s="8" t="s">
-        <v>752</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>753</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>100</v>
+      <c r="H47" s="36">
+        <v>2000.0</v>
       </c>
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="H48" s="37">
+        <v>2100.0</v>
+      </c>
+      <c r="K48" s="29" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="49" ht="13.5" customHeight="1">
+      <c r="C49" s="29" t="s">
         <v>754</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>755</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" ht="13.5" customHeight="1">
-      <c r="C49" s="8" t="s">
+      <c r="H49" s="36">
+        <v>2200.0</v>
+      </c>
+    </row>
+    <row r="50" ht="13.5" customHeight="1">
+      <c r="C50" s="29" t="s">
         <v>756</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>757</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" ht="13.5" customHeight="1">
-      <c r="C50" s="8" t="s">
-        <v>758</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>759</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>720</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>110</v>
+      <c r="H50" s="37">
+        <v>2300.0</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>761</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>720</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>113</v>
+        <v>759</v>
+      </c>
+      <c r="H51" s="36">
+        <v>2400.0</v>
+      </c>
+      <c r="K51" s="29" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>762</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="D52" s="8" t="s">
         <v>763</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>764</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>765</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>60</v>
+      <c r="H52" s="36">
+        <v>0.0</v>
       </c>
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>767</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>64</v>
+        <v>765</v>
+      </c>
+      <c r="H53" s="36">
+        <v>100.0</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>769</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>67</v>
+        <v>767</v>
+      </c>
+      <c r="H54" s="36">
+        <v>200.0</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>771</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>70</v>
+        <v>769</v>
+      </c>
+      <c r="H55" s="36">
+        <v>300.0</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1"/>
@@ -7505,23 +7476,22 @@
     <row r="999" ht="13.5" customHeight="1"/>
     <row r="1000" ht="13.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A34:A51"/>
-    <mergeCell ref="B34:B51"/>
+  <mergeCells count="9">
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B52:B55"/>
+    <mergeCell ref="A27:A51"/>
+    <mergeCell ref="B27:B51"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="A14:A26"/>
     <mergeCell ref="B14:B26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7551,7 +7521,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7602,16 +7572,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>773</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>774</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>775</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>776</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -7619,7 +7589,7 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>632</v>
@@ -7630,7 +7600,7 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>705</v>
@@ -7641,7 +7611,7 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>626</v>
@@ -7652,7 +7622,7 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>634</v>
@@ -7663,7 +7633,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>102</v>
@@ -7674,10 +7644,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -7685,19 +7655,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
+        <v>782</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>783</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>784</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>785</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>786</v>
-      </c>
       <c r="D11" s="8" t="s">
-        <v>727</v>
+        <v>716</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -7705,13 +7675,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>729</v>
+        <v>718</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -7719,13 +7689,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -7733,13 +7703,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -7747,13 +7717,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -7761,13 +7731,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -7775,13 +7745,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -7789,13 +7759,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>82</v>
@@ -7803,13 +7773,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>85</v>
@@ -7817,13 +7787,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>747</v>
+        <v>740</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>88</v>
@@ -7831,13 +7801,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>91</v>
@@ -7845,13 +7815,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>94</v>
@@ -7859,13 +7829,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>97</v>
@@ -7873,13 +7843,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>100</v>
@@ -7887,16 +7857,16 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>811</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="8" t="s">
         <v>812</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>813</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>814</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>60</v>
@@ -7904,10 +7874,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>64</v>
@@ -8929,7 +8899,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -8980,16 +8950,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -8997,10 +8967,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -9008,10 +8978,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -9019,10 +8989,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -9030,10 +9000,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -10069,7 +10039,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10120,16 +10090,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -10137,10 +10107,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
add NONRES as new occupancy atom
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="835">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -1342,6 +1342,12 @@
   </si>
   <si>
     <t>Indigenous housing</t>
+  </si>
+  <si>
+    <t>NONRES</t>
+  </si>
+  <si>
+    <t>Not residential</t>
   </si>
   <si>
     <t>COM</t>
@@ -4581,7 +4587,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4632,16 +4638,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -4649,10 +4655,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -4660,10 +4666,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -4671,10 +4677,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -4682,10 +4688,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -4693,10 +4699,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -4704,7 +4710,7 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>102</v>
@@ -4715,10 +4721,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -4726,10 +4732,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -4737,10 +4743,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -4748,10 +4754,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -4759,16 +4765,16 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>60</v>
@@ -4776,10 +4782,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>64</v>
@@ -4787,10 +4793,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>67</v>
@@ -4798,10 +4804,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>70</v>
@@ -4809,19 +4815,19 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>60</v>
@@ -4829,13 +4835,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D20" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>662</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>660</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>64</v>
@@ -5864,7 +5870,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -5915,16 +5921,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="H4" s="36">
         <v>0.0</v>
@@ -5932,10 +5938,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="H5" s="36">
         <v>100.0</v>
@@ -5943,10 +5949,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="H6" s="36">
         <v>200.0</v>
@@ -5954,10 +5960,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="H7" s="36">
         <v>300.0</v>
@@ -5965,10 +5971,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="H8" s="36">
         <v>400.0</v>
@@ -5976,10 +5982,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="H9" s="36">
         <v>500.0</v>
@@ -5987,10 +5993,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="H10" s="36">
         <v>600.0</v>
@@ -5998,10 +6004,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="H11" s="36">
         <v>700.0</v>
@@ -6009,10 +6015,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="H12" s="36">
         <v>800.0</v>
@@ -6020,10 +6026,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="H13" s="36">
         <v>900.0</v>
@@ -6031,16 +6037,16 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="H14" s="36">
         <v>0.0</v>
@@ -6048,10 +6054,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="H15" s="36">
         <v>100.0</v>
@@ -6059,10 +6065,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="H16" s="36">
         <v>200.0</v>
@@ -6070,10 +6076,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="H17" s="36">
         <v>300.0</v>
@@ -6081,7 +6087,7 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>214</v>
@@ -6092,10 +6098,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="H19" s="36">
         <v>500.0</v>
@@ -6103,10 +6109,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="H20" s="36">
         <v>600.0</v>
@@ -6114,10 +6120,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="H21" s="36">
         <v>700.0</v>
@@ -6125,10 +6131,10 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="H22" s="36">
         <v>800.0</v>
@@ -6136,10 +6142,10 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H23" s="36">
         <v>900.0</v>
@@ -6147,10 +6153,10 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="H24" s="36">
         <v>1000.0</v>
@@ -6158,10 +6164,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="H25" s="36">
         <v>1100.0</v>
@@ -6169,10 +6175,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="H26" s="36">
         <v>1200.0</v>
@@ -6180,16 +6186,16 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="32" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="H27" s="36">
         <v>0.0</v>
@@ -6200,10 +6206,10 @@
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="C28" s="29" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="H28" s="37">
         <v>100.0</v>
@@ -6211,10 +6217,10 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="C29" s="29" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H29" s="36">
         <v>200.0</v>
@@ -6222,10 +6228,10 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="C30" s="29" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="H30" s="37">
         <v>300.0</v>
@@ -6233,10 +6239,10 @@
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="C31" s="8" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H31" s="36">
         <v>400.0</v>
@@ -6247,10 +6253,10 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="C32" s="29" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="H32" s="37">
         <v>500.0</v>
@@ -6258,10 +6264,10 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="C33" s="8" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="H33" s="36">
         <v>600.0</v>
@@ -6272,10 +6278,10 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="C34" s="29" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="H34" s="37">
         <v>700.0</v>
@@ -6283,10 +6289,10 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="C35" s="29" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="H35" s="36">
         <v>800.0</v>
@@ -6294,10 +6300,10 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="29" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="H36" s="37">
         <v>900.0</v>
@@ -6305,10 +6311,10 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="C37" s="29" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="H37" s="36">
         <v>1000.0</v>
@@ -6316,10 +6322,10 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="C38" s="8" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="H38" s="37">
         <v>1100.0</v>
@@ -6330,10 +6336,10 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="C39" s="29" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="H39" s="36">
         <v>1200.0</v>
@@ -6341,10 +6347,10 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="29" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="H40" s="37">
         <v>1300.0</v>
@@ -6352,10 +6358,10 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="29" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="H41" s="36">
         <v>1400.0</v>
@@ -6363,7 +6369,7 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="C42" s="8" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>102</v>
@@ -6377,10 +6383,10 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="C43" s="29" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="H43" s="36">
         <v>1600.0</v>
@@ -6388,10 +6394,10 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="29" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H44" s="37">
         <v>1700.0</v>
@@ -6399,10 +6405,10 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="29" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="H45" s="36">
         <v>1800.0</v>
@@ -6410,10 +6416,10 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="C46" s="29" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="H46" s="37">
         <v>1900.0</v>
@@ -6421,10 +6427,10 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="29" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="H47" s="36">
         <v>2000.0</v>
@@ -6432,10 +6438,10 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="C48" s="8" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="H48" s="37">
         <v>2100.0</v>
@@ -6446,10 +6452,10 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="C49" s="29" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="H49" s="36">
         <v>2200.0</v>
@@ -6457,10 +6463,10 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="29" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="H50" s="37">
         <v>2300.0</v>
@@ -6468,10 +6474,10 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="H51" s="36">
         <v>2400.0</v>
@@ -6482,16 +6488,16 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="H52" s="36">
         <v>0.0</v>
@@ -6499,10 +6505,10 @@
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="C53" s="8" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="H53" s="36">
         <v>100.0</v>
@@ -6510,10 +6516,10 @@
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="C54" s="8" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="H54" s="36">
         <v>200.0</v>
@@ -6521,10 +6527,10 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="C55" s="8" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="H55" s="36">
         <v>300.0</v>
@@ -7521,7 +7527,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7572,16 +7578,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -7589,10 +7595,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -7600,10 +7606,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -7611,10 +7617,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -7622,10 +7628,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -7633,7 +7639,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>102</v>
@@ -7644,10 +7650,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -7655,19 +7661,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -7675,13 +7681,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -7689,13 +7695,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -7703,13 +7709,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -7717,13 +7723,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -7731,13 +7737,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -7745,13 +7751,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -7759,13 +7765,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>82</v>
@@ -7773,13 +7779,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>85</v>
@@ -7787,13 +7793,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>88</v>
@@ -7801,13 +7807,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>91</v>
@@ -7815,13 +7821,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>94</v>
@@ -7829,13 +7835,13 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>97</v>
@@ -7843,13 +7849,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="C24" s="8" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>100</v>
@@ -7857,16 +7863,16 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>60</v>
@@ -7874,10 +7880,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>64</v>
@@ -8899,7 +8905,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -8950,16 +8956,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -8967,10 +8973,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -8978,10 +8984,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -8989,10 +8995,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -9000,10 +9006,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -10039,7 +10045,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -10090,16 +10096,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -10107,10 +10113,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -50631,7 +50637,7 @@
         <v>374</v>
       </c>
       <c r="H5" s="8">
-        <f t="shared" ref="H5:H75" si="1">H4+100</f>
+        <f t="shared" ref="H5:H76" si="1">H4+100</f>
         <v>100</v>
       </c>
     </row>
@@ -50781,9 +50787,7 @@
         <f t="shared" si="1"/>
         <v>1300</v>
       </c>
-      <c r="K17" s="29" t="s">
-        <v>372</v>
-      </c>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="29" t="s">
@@ -50797,6 +50801,9 @@
         <f t="shared" si="1"/>
         <v>1400</v>
       </c>
+      <c r="K18" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="29" t="s">
@@ -50966,28 +50973,25 @@
         <f t="shared" si="1"/>
         <v>2700</v>
       </c>
-      <c r="J31" s="29" t="s">
+    </row>
+    <row r="32" ht="13.5" customHeight="1">
+      <c r="C32" s="29" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="32" ht="13.5" customHeight="1">
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="29" t="s">
         <v>428</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>429</v>
       </c>
       <c r="E32" s="29"/>
       <c r="H32" s="8">
         <f t="shared" si="1"/>
         <v>2800</v>
       </c>
-      <c r="K32" s="29" t="s">
-        <v>372</v>
+      <c r="J32" s="29" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="8" t="s">
         <v>430</v>
       </c>
       <c r="D33" s="29" t="s">
@@ -50998,6 +51002,9 @@
         <f t="shared" si="1"/>
         <v>2900</v>
       </c>
+      <c r="K33" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="C34" s="29" t="s">
@@ -51024,7 +51031,6 @@
         <f t="shared" si="1"/>
         <v>3100</v>
       </c>
-      <c r="K35" s="30"/>
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="C36" s="29" t="s">
@@ -51069,7 +51075,7 @@
       <c r="K38" s="30"/>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="29" t="s">
         <v>442</v>
       </c>
       <c r="D39" s="29" t="s">
@@ -51080,21 +51086,23 @@
         <f t="shared" si="1"/>
         <v>3500</v>
       </c>
-      <c r="K39" s="29" t="s">
-        <v>372</v>
-      </c>
+      <c r="K39" s="30"/>
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="C40" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="29" t="s">
         <v>445</v>
       </c>
+      <c r="E40" s="29"/>
       <c r="H40" s="8">
         <f t="shared" si="1"/>
         <v>3600</v>
       </c>
+      <c r="K40" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="C41" s="8" t="s">
@@ -51124,29 +51132,29 @@
       <c r="C43" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="D43" s="29" t="s">
+      <c r="D43" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="E43" s="29"/>
       <c r="H43" s="8">
         <f t="shared" si="1"/>
         <v>3900</v>
       </c>
-      <c r="K43" s="29" t="s">
-        <v>372</v>
-      </c>
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="C44" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="29" t="s">
         <v>453</v>
       </c>
+      <c r="E44" s="29"/>
       <c r="H44" s="8">
         <f t="shared" si="1"/>
         <v>4000</v>
       </c>
+      <c r="K44" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="C45" s="8" t="s">
@@ -51161,18 +51169,16 @@
       </c>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="E46" s="29"/>
       <c r="H46" s="8">
         <f t="shared" si="1"/>
         <v>4200</v>
       </c>
-      <c r="K46" s="30"/>
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="C47" s="29" t="s">
@@ -51203,7 +51209,7 @@
       <c r="K48" s="30"/>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="29" t="s">
         <v>462</v>
       </c>
       <c r="D49" s="29" t="s">
@@ -51214,21 +51220,23 @@
         <f t="shared" si="1"/>
         <v>4500</v>
       </c>
-      <c r="K49" s="29" t="s">
-        <v>372</v>
-      </c>
+      <c r="K49" s="30"/>
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="C50" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="29" t="s">
         <v>465</v>
       </c>
+      <c r="E50" s="29"/>
       <c r="H50" s="8">
         <f t="shared" si="1"/>
         <v>4600</v>
       </c>
+      <c r="K50" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="C51" s="8" t="s">
@@ -51342,29 +51350,29 @@
       <c r="C60" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="E60" s="29"/>
       <c r="H60" s="8">
         <f t="shared" si="1"/>
         <v>5600</v>
       </c>
-      <c r="K60" s="29" t="s">
-        <v>372</v>
-      </c>
     </row>
     <row r="61" ht="13.5" customHeight="1">
       <c r="C61" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="29" t="s">
         <v>487</v>
       </c>
+      <c r="E61" s="29"/>
       <c r="H61" s="8">
         <f t="shared" si="1"/>
         <v>5700</v>
       </c>
+      <c r="K61" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="C62" s="8" t="s">
@@ -51475,19 +51483,15 @@
       </c>
     </row>
     <row r="71" ht="13.5" customHeight="1">
-      <c r="C71" s="29" t="s">
+      <c r="C71" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D71" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="E71" s="29"/>
       <c r="H71" s="8">
         <f t="shared" si="1"/>
         <v>6700</v>
-      </c>
-      <c r="K71" s="29" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="72" ht="13.5" customHeight="1">
@@ -51502,6 +51506,9 @@
         <f t="shared" si="1"/>
         <v>6800</v>
       </c>
+      <c r="K72" s="29" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="C73" s="29" t="s">
@@ -51530,18 +51537,30 @@
       </c>
     </row>
     <row r="75" ht="13.5" customHeight="1">
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="D75" s="29" t="s">
         <v>515</v>
       </c>
+      <c r="E75" s="29"/>
       <c r="H75" s="8">
         <f t="shared" si="1"/>
         <v>7100</v>
       </c>
     </row>
-    <row r="76" ht="13.5" customHeight="1"/>
+    <row r="76" ht="13.5" customHeight="1">
+      <c r="C76" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="H76" s="8">
+        <f t="shared" si="1"/>
+        <v>7200</v>
+      </c>
+    </row>
     <row r="77" ht="13.5" customHeight="1"/>
     <row r="78" ht="13.5" customHeight="1"/>
     <row r="79" ht="13.5" customHeight="1"/>
@@ -52469,11 +52488,12 @@
     <row r="1001" ht="13.5" customHeight="1"/>
     <row r="1002" ht="13.5" customHeight="1"/>
     <row r="1003" ht="13.5" customHeight="1"/>
+    <row r="1004" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A4:A75"/>
-    <mergeCell ref="B4:B75"/>
+    <mergeCell ref="A4:A76"/>
+    <mergeCell ref="B4:B76"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -52508,7 +52528,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -52559,16 +52579,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -52576,10 +52596,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -52587,10 +52607,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -52598,10 +52618,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>
@@ -52609,10 +52629,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>73</v>
@@ -52620,10 +52640,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>76</v>
@@ -52631,10 +52651,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>79</v>
@@ -52642,10 +52662,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="C11" s="8" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>82</v>
@@ -52653,10 +52673,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>85</v>
@@ -52664,10 +52684,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>88</v>
@@ -52675,10 +52695,10 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>91</v>
@@ -52686,10 +52706,10 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>94</v>
@@ -52697,10 +52717,10 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>97</v>
@@ -52708,10 +52728,10 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>100</v>
@@ -52719,10 +52739,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="C18" s="8" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>103</v>
@@ -52730,10 +52750,10 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="C19" s="8" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>106</v>
@@ -52741,10 +52761,10 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="C20" s="8" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>110</v>
@@ -52752,10 +52772,10 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="C21" s="8" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>113</v>
@@ -52763,38 +52783,38 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="C22" s="8" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="C23" s="8" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>60</v>
@@ -52802,10 +52822,10 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="C25" s="8" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>64</v>
@@ -52813,10 +52833,10 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="C26" s="8" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>67</v>
@@ -52824,10 +52844,10 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="C27" s="8" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>70</v>
@@ -53847,7 +53867,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -53898,16 +53918,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -53915,10 +53935,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="33" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -53926,66 +53946,66 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>578</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>580</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>581</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>576</v>
       </c>
       <c r="H6" s="8">
         <v>0.0</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E7" s="35"/>
       <c r="F7" s="29" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="H7" s="29">
         <v>100.0</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>60</v>
@@ -53993,13 +54013,13 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="C9" s="8" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>594</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>592</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>64</v>
@@ -54007,13 +54027,13 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="C10" s="8" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>67</v>
@@ -54021,19 +54041,19 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>60</v>
@@ -54041,13 +54061,13 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="C12" s="8" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>64</v>
@@ -54055,13 +54075,13 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="C13" s="8" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>67</v>
@@ -54069,13 +54089,13 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="C14" s="8" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>70</v>
@@ -54083,13 +54103,13 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="C15" s="8" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>73</v>
@@ -54097,13 +54117,13 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="C16" s="8" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>76</v>
@@ -54111,13 +54131,13 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="C17" s="8" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>79</v>
@@ -55157,7 +55177,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -55208,16 +55228,16 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>60</v>
@@ -55225,10 +55245,10 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>64</v>
@@ -55236,10 +55256,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="C6" s="8" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>67</v>
@@ -55247,10 +55267,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="C7" s="8" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
some fix to the standard spreadsheet
</commit_message>
<xml_diff>
--- a/specs/Taxonomy_tables_v3.3.xlsx
+++ b/specs/Taxonomy_tables_v3.3.xlsx
@@ -29,6 +29,63 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D4">
+      <text>
+        <t xml:space="preserve">How can we indicate materials that change in height?
+We have cases in which the first floor is MUR and the second floor are metal sheets (INF)
+Options:
+1) We add the attribute MDV: Different materials in in height.
+MDV(MUR,INF)
+2) We modify the description of the MDD to be
+"Different materials in the two directions or in height"
+NOTE: For the LLRS we have LDD and LHV.
+In case we go for option2, the LLRS could be the one indicating the differences (LDD for direction and LHV for heights)
+	-Catalina YepesE
+Any preference?
+@anirudh.rao@globalquakemodel.org
+	-Catalina YepesE</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="D17">
+      <text>
+        <t xml:space="preserve">When and how would we use the NONRES occupancy?  This seems very odd, we do not have NONCOM or other negated occupancy or construction classes, and it is already possible to specify mixed occupancy or other.   Does it make sense to have  a vulnerability curve for a NONRES taxonomy?
+	-Paul Henshaw
+Thank you Paul.
+You are correct that this is not not ideal.
+However, we have in the GRM the case in which the occupancy is explicitly indicated as non residential.
+Do you have any idea?
+The MIX wont work because are not multiple occupancy types.
+Regarding the vulnerability, the taxonomy is not directly applied to the vulnerability. In the cases when NONRES appear, we do a mapping to IND/COM to assign possible vulnerability functions (for the specific case of the GRM)
+	-Catalina YepesE
+So why is this not equivalent to MIX(IND,COM), at least in the context of the GRM?
+	-Paul Henshaw
+Because it's not that the building has mixed used.
+Some of the models include mixed, specially for RES and COM (e.g., first stories commercial and upper floors residential)
+	-Catalina YepesE
+It seems to me that this introduces a concept of uncertainty just for one kind of occupancy: with NONRES meaning "we don't know what occupancy this is but it's not residential"; we do not have any similar language construct for any other element of the taxonomy.   This seems asymmetric.
+	-Paul Henshaw</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="A27">
       <text>
         <t xml:space="preserve">@catalina.yepes@globalquakemodel.org  my proposal is merge material and type together using the same approach used for occupancy:
@@ -42,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="835">
   <si>
     <t>Taxonomy 3.3: Summary</t>
   </si>
@@ -2205,7 +2262,7 @@
     <t>RSH7</t>
   </si>
   <si>
-    <t xml:space="preserve"> Curved</t>
+    <t>Curved</t>
   </si>
   <si>
     <t>RSH8</t>
@@ -2397,7 +2454,7 @@
     <t>RWO:1</t>
   </si>
   <si>
-    <t>Wooden structurewith light roof covering</t>
+    <t>Wooden structure with light roof covering</t>
   </si>
   <si>
     <t>RWO:2</t>
@@ -2671,7 +2728,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -2711,6 +2768,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2765,7 +2827,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2867,6 +2929,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -4526,11 +4591,11 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="B31:B35"/>
     <mergeCell ref="C31:C35"/>
@@ -4600,7 +4665,9 @@
       <c r="J1" s="2"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1"/>
+    <row r="2" ht="13.5" customHeight="1">
+      <c r="D2" s="36"/>
+    </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>45</v>
@@ -5932,7 +5999,7 @@
       <c r="D4" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="37">
         <v>0.0</v>
       </c>
     </row>
@@ -5943,7 +6010,7 @@
       <c r="D5" s="8" t="s">
         <v>671</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="37">
         <v>100.0</v>
       </c>
     </row>
@@ -5954,7 +6021,7 @@
       <c r="D6" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -5965,7 +6032,7 @@
       <c r="D7" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="37">
         <v>300.0</v>
       </c>
     </row>
@@ -5976,7 +6043,7 @@
       <c r="D8" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="37">
         <v>400.0</v>
       </c>
     </row>
@@ -5987,7 +6054,7 @@
       <c r="D9" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="37">
         <v>500.0</v>
       </c>
     </row>
@@ -5995,10 +6062,10 @@
       <c r="C10" s="8" t="s">
         <v>680</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="29" t="s">
         <v>681</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="37">
         <v>600.0</v>
       </c>
     </row>
@@ -6009,7 +6076,7 @@
       <c r="D11" s="8" t="s">
         <v>683</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="37">
         <v>700.0</v>
       </c>
     </row>
@@ -6020,7 +6087,7 @@
       <c r="D12" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="37">
         <v>800.0</v>
       </c>
     </row>
@@ -6031,7 +6098,7 @@
       <c r="D13" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="37">
         <v>900.0</v>
       </c>
     </row>
@@ -6048,7 +6115,7 @@
       <c r="D14" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="37">
         <v>0.0</v>
       </c>
     </row>
@@ -6059,7 +6126,7 @@
       <c r="D15" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="37">
         <v>100.0</v>
       </c>
     </row>
@@ -6070,7 +6137,7 @@
       <c r="D16" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -6081,7 +6148,7 @@
       <c r="D17" s="8" t="s">
         <v>697</v>
       </c>
-      <c r="H17" s="36">
+      <c r="H17" s="37">
         <v>300.0</v>
       </c>
     </row>
@@ -6092,7 +6159,7 @@
       <c r="D18" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="37">
         <v>400.0</v>
       </c>
     </row>
@@ -6103,7 +6170,7 @@
       <c r="D19" s="8" t="s">
         <v>700</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H19" s="37">
         <v>500.0</v>
       </c>
     </row>
@@ -6114,7 +6181,7 @@
       <c r="D20" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="37">
         <v>600.0</v>
       </c>
     </row>
@@ -6125,7 +6192,7 @@
       <c r="D21" s="8" t="s">
         <v>704</v>
       </c>
-      <c r="H21" s="36">
+      <c r="H21" s="37">
         <v>700.0</v>
       </c>
     </row>
@@ -6136,7 +6203,7 @@
       <c r="D22" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="H22" s="36">
+      <c r="H22" s="37">
         <v>800.0</v>
       </c>
     </row>
@@ -6147,7 +6214,7 @@
       <c r="D23" s="8" t="s">
         <v>707</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="37">
         <v>900.0</v>
       </c>
     </row>
@@ -6158,7 +6225,7 @@
       <c r="D24" s="8" t="s">
         <v>709</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="37">
         <v>1000.0</v>
       </c>
     </row>
@@ -6169,7 +6236,7 @@
       <c r="D25" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="H25" s="36">
+      <c r="H25" s="37">
         <v>1100.0</v>
       </c>
     </row>
@@ -6180,7 +6247,7 @@
       <c r="D26" s="8" t="s">
         <v>713</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="37">
         <v>1200.0</v>
       </c>
     </row>
@@ -6197,7 +6264,7 @@
       <c r="D27" s="8" t="s">
         <v>634</v>
       </c>
-      <c r="H27" s="36">
+      <c r="H27" s="37">
         <v>0.0</v>
       </c>
       <c r="K27" s="29" t="s">
@@ -6211,7 +6278,7 @@
       <c r="D28" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="H28" s="37">
+      <c r="H28" s="38">
         <v>100.0</v>
       </c>
     </row>
@@ -6222,7 +6289,7 @@
       <c r="D29" s="8" t="s">
         <v>720</v>
       </c>
-      <c r="H29" s="36">
+      <c r="H29" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -6233,7 +6300,7 @@
       <c r="D30" s="8" t="s">
         <v>722</v>
       </c>
-      <c r="H30" s="37">
+      <c r="H30" s="38">
         <v>300.0</v>
       </c>
     </row>
@@ -6244,7 +6311,7 @@
       <c r="D31" s="8" t="s">
         <v>707</v>
       </c>
-      <c r="H31" s="36">
+      <c r="H31" s="37">
         <v>400.0</v>
       </c>
       <c r="K31" s="29" t="s">
@@ -6258,7 +6325,7 @@
       <c r="D32" s="8" t="s">
         <v>725</v>
       </c>
-      <c r="H32" s="37">
+      <c r="H32" s="38">
         <v>500.0</v>
       </c>
     </row>
@@ -6269,7 +6336,7 @@
       <c r="D33" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H33" s="37">
         <v>600.0</v>
       </c>
       <c r="K33" s="29" t="s">
@@ -6283,7 +6350,7 @@
       <c r="D34" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="H34" s="37">
+      <c r="H34" s="38">
         <v>700.0</v>
       </c>
     </row>
@@ -6294,7 +6361,7 @@
       <c r="D35" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H35" s="37">
         <v>800.0</v>
       </c>
     </row>
@@ -6305,7 +6372,7 @@
       <c r="D36" s="8" t="s">
         <v>732</v>
       </c>
-      <c r="H36" s="37">
+      <c r="H36" s="38">
         <v>900.0</v>
       </c>
     </row>
@@ -6316,7 +6383,7 @@
       <c r="D37" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="H37" s="36">
+      <c r="H37" s="37">
         <v>1000.0</v>
       </c>
     </row>
@@ -6327,7 +6394,7 @@
       <c r="D38" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="H38" s="37">
+      <c r="H38" s="38">
         <v>1100.0</v>
       </c>
       <c r="K38" s="29" t="s">
@@ -6341,7 +6408,7 @@
       <c r="D39" s="8" t="s">
         <v>738</v>
       </c>
-      <c r="H39" s="36">
+      <c r="H39" s="37">
         <v>1200.0</v>
       </c>
     </row>
@@ -6352,7 +6419,7 @@
       <c r="D40" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="H40" s="37">
+      <c r="H40" s="38">
         <v>1300.0</v>
       </c>
     </row>
@@ -6363,7 +6430,7 @@
       <c r="D41" s="8" t="s">
         <v>742</v>
       </c>
-      <c r="H41" s="36">
+      <c r="H41" s="37">
         <v>1400.0</v>
       </c>
     </row>
@@ -6374,7 +6441,7 @@
       <c r="D42" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H42" s="37">
+      <c r="H42" s="38">
         <v>1500.0</v>
       </c>
       <c r="K42" s="29" t="s">
@@ -6385,10 +6452,10 @@
       <c r="C43" s="29" t="s">
         <v>744</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="29" t="s">
         <v>745</v>
       </c>
-      <c r="H43" s="36">
+      <c r="H43" s="37">
         <v>1600.0</v>
       </c>
     </row>
@@ -6399,7 +6466,7 @@
       <c r="D44" s="8" t="s">
         <v>747</v>
       </c>
-      <c r="H44" s="37">
+      <c r="H44" s="38">
         <v>1700.0</v>
       </c>
     </row>
@@ -6410,7 +6477,7 @@
       <c r="D45" s="8" t="s">
         <v>749</v>
       </c>
-      <c r="H45" s="36">
+      <c r="H45" s="37">
         <v>1800.0</v>
       </c>
     </row>
@@ -6421,7 +6488,7 @@
       <c r="D46" s="8" t="s">
         <v>751</v>
       </c>
-      <c r="H46" s="37">
+      <c r="H46" s="38">
         <v>1900.0</v>
       </c>
     </row>
@@ -6432,7 +6499,7 @@
       <c r="D47" s="8" t="s">
         <v>753</v>
       </c>
-      <c r="H47" s="36">
+      <c r="H47" s="37">
         <v>2000.0</v>
       </c>
     </row>
@@ -6443,7 +6510,7 @@
       <c r="D48" s="8" t="s">
         <v>755</v>
       </c>
-      <c r="H48" s="37">
+      <c r="H48" s="38">
         <v>2100.0</v>
       </c>
       <c r="K48" s="29" t="s">
@@ -6457,7 +6524,7 @@
       <c r="D49" s="8" t="s">
         <v>757</v>
       </c>
-      <c r="H49" s="36">
+      <c r="H49" s="37">
         <v>2200.0</v>
       </c>
     </row>
@@ -6468,7 +6535,7 @@
       <c r="D50" s="8" t="s">
         <v>759</v>
       </c>
-      <c r="H50" s="37">
+      <c r="H50" s="38">
         <v>2300.0</v>
       </c>
     </row>
@@ -6479,12 +6546,10 @@
       <c r="D51" s="8" t="s">
         <v>761</v>
       </c>
-      <c r="H51" s="36">
+      <c r="H51" s="37">
         <v>2400.0</v>
       </c>
-      <c r="K51" s="29" t="s">
-        <v>372</v>
-      </c>
+      <c r="K51" s="29"/>
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="6" t="s">
@@ -6499,7 +6564,7 @@
       <c r="D52" s="8" t="s">
         <v>765</v>
       </c>
-      <c r="H52" s="36">
+      <c r="H52" s="38">
         <v>0.0</v>
       </c>
     </row>
@@ -6510,7 +6575,7 @@
       <c r="D53" s="8" t="s">
         <v>767</v>
       </c>
-      <c r="H53" s="36">
+      <c r="H53" s="37">
         <v>100.0</v>
       </c>
     </row>
@@ -6521,7 +6586,7 @@
       <c r="D54" s="8" t="s">
         <v>769</v>
       </c>
-      <c r="H54" s="36">
+      <c r="H54" s="37">
         <v>200.0</v>
       </c>
     </row>
@@ -6532,7 +6597,7 @@
       <c r="D55" s="8" t="s">
         <v>771</v>
       </c>
-      <c r="H55" s="36">
+      <c r="H55" s="37">
         <v>300.0</v>
       </c>
     </row>
@@ -7485,13 +7550,13 @@
   <mergeCells count="9">
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B52:B55"/>
-    <mergeCell ref="A27:A51"/>
-    <mergeCell ref="B27:B51"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="A14:A26"/>
     <mergeCell ref="B14:B26"/>
+    <mergeCell ref="A27:A51"/>
+    <mergeCell ref="B27:B51"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -15933,7 +15998,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -50545,7 +50611,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="23.43"/>
     <col customWidth="1" min="2" max="2" width="31.43"/>
-    <col customWidth="1" min="3" max="3" width="11.43"/>
+    <col customWidth="1" min="3" max="3" width="9.29"/>
     <col customWidth="1" min="4" max="4" width="44.43"/>
     <col customWidth="1" min="5" max="5" width="16.29"/>
     <col customWidth="1" min="6" max="6" width="13.71"/>
@@ -52498,7 +52564,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>